<commit_message>
programação para o whatsapp
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A977C82-31F4-428F-84DB-0AE205276FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7B9300-BA61-469E-ACD4-DBF1BB37654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programacao" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="230">
   <si>
     <t>Data de Entrada</t>
   </si>
@@ -267,6 +267,123 @@
     <t>JBD6C75</t>
   </si>
   <si>
+    <t>11/02/2025</t>
+  </si>
+  <si>
+    <t>06:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRUNO TEIXEIRA </t>
+  </si>
+  <si>
+    <t>(11)9470374018</t>
+  </si>
+  <si>
+    <t>124603</t>
+  </si>
+  <si>
+    <t>BWP0349</t>
+  </si>
+  <si>
+    <t>COMPLEX</t>
+  </si>
+  <si>
+    <t>19:08</t>
+  </si>
+  <si>
+    <t>12/02/2025</t>
+  </si>
+  <si>
+    <t>07:13</t>
+  </si>
+  <si>
+    <t>ALEXANDRE DA SILVA BONIFACIO</t>
+  </si>
+  <si>
+    <t>(11)988985465</t>
+  </si>
+  <si>
+    <t>355674</t>
+  </si>
+  <si>
+    <t>EPU8B65</t>
+  </si>
+  <si>
+    <t>NOVO MUNDO</t>
+  </si>
+  <si>
+    <t>07:22</t>
+  </si>
+  <si>
+    <t>NIVALDO</t>
+  </si>
+  <si>
+    <t>354836</t>
+  </si>
+  <si>
+    <t>NFF7E78</t>
+  </si>
+  <si>
+    <t>08:39</t>
+  </si>
+  <si>
+    <t>WALTER DE LIRA MIRANDA</t>
+  </si>
+  <si>
+    <t>(1)957288223</t>
+  </si>
+  <si>
+    <t>354401</t>
+  </si>
+  <si>
+    <t>ATM4876</t>
+  </si>
+  <si>
+    <t>08:28</t>
+  </si>
+  <si>
+    <t>MAURICIO TIAGO IZIDORO</t>
+  </si>
+  <si>
+    <t>(43)996860461</t>
+  </si>
+  <si>
+    <t>654742</t>
+  </si>
+  <si>
+    <t>USINA ALTA MOGIANA</t>
+  </si>
+  <si>
+    <t>QKL3C74</t>
+  </si>
+  <si>
+    <t>SAIDER</t>
+  </si>
+  <si>
+    <t>AÇUCAR+EMBALAGEM 1200KG</t>
+  </si>
+  <si>
+    <t>LANCHOTE TRENSPORTES</t>
+  </si>
+  <si>
+    <t>08:56</t>
+  </si>
+  <si>
+    <t>RAFAEL DE PAULA RODRIGES</t>
+  </si>
+  <si>
+    <t>(16)981320861</t>
+  </si>
+  <si>
+    <t>654739</t>
+  </si>
+  <si>
+    <t>DAO0375</t>
+  </si>
+  <si>
+    <t>LANCHOTE TRANSPORTES</t>
+  </si>
+  <si>
     <t>Movimento</t>
   </si>
   <si>
@@ -417,6 +534,63 @@
     <t>355507</t>
   </si>
   <si>
+    <t>124604</t>
+  </si>
+  <si>
+    <t>25010232</t>
+  </si>
+  <si>
+    <t>25010212</t>
+  </si>
+  <si>
+    <t>354673</t>
+  </si>
+  <si>
+    <t>354676</t>
+  </si>
+  <si>
+    <t>354675</t>
+  </si>
+  <si>
+    <t>354835</t>
+  </si>
+  <si>
+    <t>354838</t>
+  </si>
+  <si>
+    <t>354837</t>
+  </si>
+  <si>
+    <t>354400</t>
+  </si>
+  <si>
+    <t>354403</t>
+  </si>
+  <si>
+    <t>354402</t>
+  </si>
+  <si>
+    <t>AÇUCAR+EMBALAGEM</t>
+  </si>
+  <si>
+    <t>1200KG</t>
+  </si>
+  <si>
+    <t>760</t>
+  </si>
+  <si>
+    <t>359</t>
+  </si>
+  <si>
+    <t>jul/26</t>
+  </si>
+  <si>
+    <t>761</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
     <t>DESCARGA DE SAL</t>
   </si>
   <si>
@@ -459,6 +633,9 @@
     <t>NF 2 FORNECEDOR:</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>NF 2 PALETE:</t>
   </si>
   <si>
@@ -490,9 +667,6 @@
   </si>
   <si>
     <t>LOTE AJIN.</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>CONFERÊNCIA</t>
@@ -833,28 +1007,47 @@
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -864,44 +1057,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1258,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,6 +1838,251 @@
         <v>65</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>18200</v>
+      </c>
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13">
+        <v>6750</v>
+      </c>
+      <c r="H13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14">
+        <v>14850</v>
+      </c>
+      <c r="H14" t="s">
+        <v>94</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>14850</v>
+      </c>
+      <c r="H15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>51</v>
+      </c>
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16">
+        <v>22950</v>
+      </c>
+      <c r="H16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" t="s">
+        <v>28</v>
+      </c>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17">
+        <v>33600</v>
+      </c>
+      <c r="H17" t="s">
+        <v>110</v>
+      </c>
+      <c r="I17" t="s">
+        <v>111</v>
+      </c>
+      <c r="J17" t="s">
+        <v>112</v>
+      </c>
+      <c r="K17" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18">
+        <v>31200</v>
+      </c>
+      <c r="H18" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+      <c r="J18" t="s">
+        <v>112</v>
+      </c>
+      <c r="K18" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1671,10 +2090,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD19"/>
+      <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1683,7 +2102,7 @@
     <col min="2" max="2" width="11.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -1691,15 +2110,15 @@
     <col min="10" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1711,36 +2130,36 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>122</v>
       </c>
       <c r="G1" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="J1" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="K1" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="L1" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
       <c r="M1" t="s">
-        <v>89</v>
+        <v>128</v>
       </c>
       <c r="N1" t="s">
-        <v>90</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -1755,10 +2174,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -1767,16 +2186,16 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>94</v>
+        <v>133</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="M2" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N2">
         <v>28000</v>
@@ -1784,7 +2203,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -1799,10 +2218,10 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G3" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -1811,16 +2230,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>98</v>
+        <v>137</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="M3" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N3">
         <v>27000</v>
@@ -1828,7 +2247,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -1843,10 +2262,10 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -1855,16 +2274,16 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>100</v>
+        <v>139</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>101</v>
+        <v>140</v>
       </c>
       <c r="M4" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N4">
         <v>6750</v>
@@ -1872,7 +2291,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -1887,28 +2306,28 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G5" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>102</v>
+        <v>141</v>
       </c>
       <c r="J5" t="s">
-        <v>103</v>
+        <v>142</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>99</v>
+        <v>138</v>
       </c>
       <c r="M5" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N5">
         <v>20250</v>
@@ -1916,7 +2335,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -1943,16 +2362,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>105</v>
+        <v>144</v>
       </c>
       <c r="M6" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="N6">
         <v>4200</v>
@@ -1960,7 +2379,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -1987,16 +2406,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>104</v>
+        <v>143</v>
       </c>
       <c r="K7">
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>107</v>
+        <v>146</v>
       </c>
       <c r="M7" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="N7">
         <v>28000</v>
@@ -2004,7 +2423,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2019,10 +2438,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G8" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2031,16 +2450,16 @@
         <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>109</v>
+        <v>148</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>110</v>
+        <v>149</v>
       </c>
       <c r="M8" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N8">
         <v>2700</v>
@@ -2048,7 +2467,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2063,28 +2482,28 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G9" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>111</v>
+        <v>150</v>
       </c>
       <c r="J9" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="K9">
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="M9" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N9">
         <v>22950</v>
@@ -2092,7 +2511,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -2107,10 +2526,10 @@
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -2119,16 +2538,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="K10">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="M10" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N10">
         <v>16200</v>
@@ -2136,7 +2555,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -2151,28 +2570,28 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>155</v>
       </c>
       <c r="J11" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="K11">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="M11" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N11">
         <v>32400</v>
@@ -2180,7 +2599,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -2195,10 +2614,10 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G12" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -2207,16 +2626,16 @@
         <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>118</v>
+        <v>157</v>
       </c>
       <c r="K12">
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="M12" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N12">
         <v>5400</v>
@@ -2224,7 +2643,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -2239,28 +2658,28 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>159</v>
       </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="M13" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N13">
         <v>24300</v>
@@ -2268,7 +2687,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -2283,10 +2702,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G14" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
@@ -2295,16 +2714,16 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>122</v>
+        <v>161</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="M14" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N14">
         <v>25650</v>
@@ -2312,7 +2731,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -2327,10 +2746,10 @@
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>92</v>
+        <v>131</v>
       </c>
       <c r="G15" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
@@ -2339,16 +2758,16 @@
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>124</v>
+        <v>163</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="M15" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="N15">
         <v>25650</v>
@@ -2356,7 +2775,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -2371,10 +2790,10 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G16" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
@@ -2383,16 +2802,16 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="N16">
         <v>1350</v>
@@ -2400,7 +2819,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -2415,31 +2834,559 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>108</v>
+        <v>147</v>
       </c>
       <c r="G17" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>129</v>
+        <v>168</v>
       </c>
       <c r="J17" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="M17" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
       <c r="N17">
         <v>28350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
+        <v>85</v>
+      </c>
+      <c r="J18" t="s">
+        <v>170</v>
+      </c>
+      <c r="K18">
+        <v>13</v>
+      </c>
+      <c r="L18" t="s">
+        <v>171</v>
+      </c>
+      <c r="M18" t="s">
+        <v>135</v>
+      </c>
+      <c r="N18">
+        <v>18200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>130</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" t="s">
+        <v>131</v>
+      </c>
+      <c r="G19" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" t="s">
+        <v>170</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19" t="s">
+        <v>172</v>
+      </c>
+      <c r="M19" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" t="s">
+        <v>131</v>
+      </c>
+      <c r="G20" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" t="s">
+        <v>139</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20" t="s">
+        <v>140</v>
+      </c>
+      <c r="M20" t="s">
+        <v>135</v>
+      </c>
+      <c r="N20">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21">
+        <v>15</v>
+      </c>
+      <c r="L21" t="s">
+        <v>138</v>
+      </c>
+      <c r="M21" t="s">
+        <v>135</v>
+      </c>
+      <c r="N21">
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>130</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I22" t="s">
+        <v>93</v>
+      </c>
+      <c r="J22" t="s">
+        <v>173</v>
+      </c>
+      <c r="K22">
+        <v>11</v>
+      </c>
+      <c r="L22" t="s">
+        <v>162</v>
+      </c>
+      <c r="M22" t="s">
+        <v>135</v>
+      </c>
+      <c r="N22">
+        <v>14850</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" t="s">
+        <v>131</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" t="s">
+        <v>174</v>
+      </c>
+      <c r="J23" t="s">
+        <v>175</v>
+      </c>
+      <c r="K23">
+        <v>8</v>
+      </c>
+      <c r="L23" t="s">
+        <v>164</v>
+      </c>
+      <c r="M23" t="s">
+        <v>135</v>
+      </c>
+      <c r="N23">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" t="s">
+        <v>132</v>
+      </c>
+      <c r="H24" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" t="s">
+        <v>98</v>
+      </c>
+      <c r="J24" t="s">
+        <v>176</v>
+      </c>
+      <c r="K24">
+        <v>11</v>
+      </c>
+      <c r="L24" t="s">
+        <v>149</v>
+      </c>
+      <c r="M24" t="s">
+        <v>135</v>
+      </c>
+      <c r="N24">
+        <v>14850</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>130</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>99</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" t="s">
+        <v>132</v>
+      </c>
+      <c r="H25" t="s">
+        <v>26</v>
+      </c>
+      <c r="I25" t="s">
+        <v>177</v>
+      </c>
+      <c r="J25" t="s">
+        <v>178</v>
+      </c>
+      <c r="K25">
+        <v>8</v>
+      </c>
+      <c r="L25" t="s">
+        <v>158</v>
+      </c>
+      <c r="M25" t="s">
+        <v>135</v>
+      </c>
+      <c r="N25">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" t="s">
+        <v>132</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" t="s">
+        <v>103</v>
+      </c>
+      <c r="J26" t="s">
+        <v>179</v>
+      </c>
+      <c r="K26">
+        <v>17</v>
+      </c>
+      <c r="L26" t="s">
+        <v>164</v>
+      </c>
+      <c r="M26" t="s">
+        <v>135</v>
+      </c>
+      <c r="N26">
+        <v>22950</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" t="s">
+        <v>26</v>
+      </c>
+      <c r="I27" t="s">
+        <v>180</v>
+      </c>
+      <c r="J27" t="s">
+        <v>181</v>
+      </c>
+      <c r="K27">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>162</v>
+      </c>
+      <c r="M27" t="s">
+        <v>135</v>
+      </c>
+      <c r="N27">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>110</v>
+      </c>
+      <c r="D28" t="s">
+        <v>111</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" t="s">
+        <v>182</v>
+      </c>
+      <c r="G28" t="s">
+        <v>183</v>
+      </c>
+      <c r="H28" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" t="s">
+        <v>108</v>
+      </c>
+      <c r="J28" t="s">
+        <v>184</v>
+      </c>
+      <c r="K28">
+        <v>28</v>
+      </c>
+      <c r="L28" t="s">
+        <v>185</v>
+      </c>
+      <c r="M28" t="s">
+        <v>186</v>
+      </c>
+      <c r="N28">
+        <v>33600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" t="s">
+        <v>89</v>
+      </c>
+      <c r="C29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D29" t="s">
+        <v>111</v>
+      </c>
+      <c r="E29" t="s">
+        <v>119</v>
+      </c>
+      <c r="F29" t="s">
+        <v>182</v>
+      </c>
+      <c r="G29" t="s">
+        <v>183</v>
+      </c>
+      <c r="H29" t="s">
+        <v>109</v>
+      </c>
+      <c r="I29" t="s">
+        <v>117</v>
+      </c>
+      <c r="J29" t="s">
+        <v>187</v>
+      </c>
+      <c r="K29">
+        <v>26</v>
+      </c>
+      <c r="L29" t="s">
+        <v>188</v>
+      </c>
+      <c r="M29" t="s">
+        <v>186</v>
+      </c>
+      <c r="N29">
+        <v>31200</v>
       </c>
     </row>
   </sheetData>
@@ -2451,7 +3398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K22" sqref="K22:N23"/>
     </sheetView>
   </sheetViews>
@@ -2476,1132 +3423,1222 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="30"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="16"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="17"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="18"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="17"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="18"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="17"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="18"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="21"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="28"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="4"/>
+      <c r="B8" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8" s="7"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="5"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="5"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="4"/>
+      <c r="B10" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="3"/>
       <c r="D10" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="5"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C12" s="4"/>
+      <c r="B12" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C12" s="3"/>
       <c r="D12" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="4"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="3"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="5"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" s="4"/>
+      <c r="B14" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="4"/>
+        <v>118</v>
+      </c>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="5"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="5"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C16" s="4"/>
+      <c r="B16" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="3"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="5"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="5"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C18" s="4"/>
+      <c r="B18" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B19" s="8"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="5"/>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B20" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="I20" s="7"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="P20" s="13">
+        <v>31200</v>
+      </c>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B21" s="8"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="14"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="5"/>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B22" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="I22" s="7"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="5"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B24" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I24" s="7"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="14"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="5"/>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B26" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="13" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="K26" s="3"/>
+      <c r="L26" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="8"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="5"/>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B28" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="I28" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="J28" s="3"/>
+      <c r="K28" s="13">
+        <v>31200</v>
+      </c>
+      <c r="L28" s="3"/>
+      <c r="M28" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="N28" s="7"/>
+      <c r="O28" s="13">
         <v>26</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="K18" s="3"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="4"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="5"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="7"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I20" s="3"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="13">
-        <v>355505</v>
-      </c>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="P20" s="13">
-        <v>1350</v>
-      </c>
-      <c r="Q20" s="4"/>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="5"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="7"/>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="I22" s="3"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="13">
-        <v>355507</v>
-      </c>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="P22" s="13">
-        <v>28350</v>
-      </c>
-      <c r="Q22" s="4"/>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="5"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="5"/>
-      <c r="Q23" s="7"/>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="I24" s="3"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="4"/>
-      <c r="O24" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="4"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="5"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="7"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="5"/>
-      <c r="Q25" s="7"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="K26" s="4"/>
-      <c r="L26" s="32" t="s">
-        <v>128</v>
-      </c>
-      <c r="M26" s="3"/>
-      <c r="N26" s="3"/>
-      <c r="O26" s="3"/>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="4"/>
-    </row>
-    <row r="27" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="5"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="6"/>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="7"/>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E28" s="8" t="s">
+      <c r="P28" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q28" s="33"/>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="14"/>
+      <c r="P29" s="14"/>
+      <c r="Q29" s="14"/>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B30" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J28" s="4"/>
-      <c r="K28" s="13">
-        <v>1350</v>
-      </c>
-      <c r="L28" s="4"/>
-      <c r="M28" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="13">
-        <v>1</v>
-      </c>
-      <c r="P28" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q28" s="25"/>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="5"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="7"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="23"/>
-      <c r="P29" s="23"/>
-      <c r="Q29" s="23"/>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B30" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E30" s="8" t="s">
+      <c r="F30" s="7"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="I30" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="J30" s="3"/>
+      <c r="K30" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="L30" s="3"/>
+      <c r="M30" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="N30" s="7"/>
+      <c r="O30" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="P30" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q30" s="33"/>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B31" s="8"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B32" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="3"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J30" s="4"/>
-      <c r="K30" s="13">
-        <v>28350</v>
-      </c>
-      <c r="L30" s="4"/>
-      <c r="M30" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="N30" s="3"/>
-      <c r="O30" s="13">
-        <v>21</v>
-      </c>
-      <c r="P30" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="Q30" s="25"/>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B31" s="5"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="7"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="6"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="4"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="3"/>
       <c r="H32" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="J32" s="4"/>
+        <v>203</v>
+      </c>
+      <c r="I32" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="J32" s="3"/>
       <c r="K32" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="L32" s="4"/>
-      <c r="M32" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="N32" s="3"/>
+        <v>203</v>
+      </c>
+      <c r="L32" s="3"/>
+      <c r="M32" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="N32" s="7"/>
       <c r="O32" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="P32" s="29" t="s">
-        <v>155</v>
+        <v>203</v>
+      </c>
+      <c r="P32" s="16" t="s">
+        <v>214</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B33" s="5"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="23"/>
-      <c r="P33" s="23"/>
-      <c r="Q33" s="23"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="14"/>
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14"/>
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="16"/>
+      <c r="B35" s="32" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="22"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="23"/>
     </row>
     <row r="36" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="19"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="21"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="27"/>
+      <c r="Q36" s="28"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B38" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C38" s="4"/>
+      <c r="B38" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C38" s="3"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38" s="4"/>
+      <c r="E38" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="3"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="L38" s="4"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="4"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="L38" s="3"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="3"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B39" s="5"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="7"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="7"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="8"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="8"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="5"/>
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="C40" s="4"/>
+      <c r="B40" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="4"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="4"/>
-      <c r="K40" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="L40" s="4"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="4"/>
+      <c r="E40" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="L40" s="3"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="3"/>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B41" s="5"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="6"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="7"/>
+      <c r="B41" s="8"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="5"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B42" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="C42" s="4"/>
+      <c r="B42" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L42" s="4"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="L42" s="3"/>
       <c r="M42" s="13"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="4"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="3"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B43" s="5"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="7"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="8"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="5"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B44" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H44" s="4"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="4"/>
+      <c r="B44" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="19" t="s">
+        <v>225</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="3"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="3"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B45" s="10"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="12"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="12"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="7"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="7"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="8"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="5"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B46" s="10"/>
+      <c r="B46" s="11"/>
       <c r="C46" s="12"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="4"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="H46" s="3"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="7"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="3"/>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B47" s="10"/>
+      <c r="B47" s="11"/>
       <c r="C47" s="12"/>
-      <c r="D47" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="7"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="5"/>
-      <c r="Q47" s="7"/>
+      <c r="D47" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="E47" s="7"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="8"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="5"/>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B48" s="10"/>
+      <c r="B48" s="11"/>
       <c r="C48" s="12"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="4"/>
+      <c r="G48" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="H48" s="3"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="7"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="3"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B49" s="5"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="7"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="5"/>
-      <c r="Q49" s="7"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="8"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="5"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="5"/>
     </row>
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B51" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="15"/>
-      <c r="F51" s="15"/>
-      <c r="G51" s="15"/>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="16"/>
+      <c r="B51" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="C51" s="22"/>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="H51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
+      <c r="K51" s="22"/>
+      <c r="L51" s="22"/>
+      <c r="M51" s="22"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
+      <c r="P51" s="22"/>
+      <c r="Q51" s="23"/>
     </row>
     <row r="52" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="19"/>
-      <c r="C52" s="20"/>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="L52" s="20"/>
-      <c r="M52" s="20"/>
-      <c r="N52" s="20"/>
-      <c r="O52" s="20"/>
-      <c r="P52" s="20"/>
-      <c r="Q52" s="21"/>
+      <c r="B52" s="26"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
+      <c r="E52" s="27"/>
+      <c r="F52" s="27"/>
+      <c r="G52" s="27"/>
+      <c r="H52" s="27"/>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+      <c r="N52" s="27"/>
+      <c r="O52" s="27"/>
+      <c r="P52" s="27"/>
+      <c r="Q52" s="28"/>
     </row>
     <row r="53" spans="2:17" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B54" s="13"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="4"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="3"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B55" s="10"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
       <c r="Q55" s="12"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B56" s="10"/>
-      <c r="C56" s="11"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
       <c r="Q56" s="12"/>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B57" s="10"/>
-      <c r="C57" s="11"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="20"/>
       <c r="Q57" s="12"/>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B58" s="10"/>
-      <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
       <c r="Q58" s="12"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B59" s="5"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="6"/>
-      <c r="N59" s="6"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
-      <c r="Q59" s="7"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4"/>
+      <c r="Q59" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="M40:Q41"/>
+    <mergeCell ref="H20:J21"/>
+    <mergeCell ref="D47:F49"/>
+    <mergeCell ref="K42:L43"/>
+    <mergeCell ref="K28:L29"/>
+    <mergeCell ref="P24:Q25"/>
+    <mergeCell ref="F2:Q6"/>
+    <mergeCell ref="B32:C33"/>
+    <mergeCell ref="G44:H45"/>
+    <mergeCell ref="M38:Q39"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="H32:H33"/>
+    <mergeCell ref="K8:Q9"/>
+    <mergeCell ref="B26:C27"/>
+    <mergeCell ref="D42:J43"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="I30:J31"/>
+    <mergeCell ref="K30:L31"/>
+    <mergeCell ref="B8:C9"/>
+    <mergeCell ref="L46:O47"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="Q28:Q29"/>
+    <mergeCell ref="J18:L19"/>
+    <mergeCell ref="L48:O49"/>
+    <mergeCell ref="B51:Q52"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="H12:J13"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="B35:Q36"/>
+    <mergeCell ref="B54:Q59"/>
+    <mergeCell ref="H14:J15"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P48:Q49"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K22:N23"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="H38:J39"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D24:G25"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="H40:J41"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="P20:Q21"/>
+    <mergeCell ref="E28:G29"/>
+    <mergeCell ref="I32:J33"/>
+    <mergeCell ref="B2:E6"/>
+    <mergeCell ref="H22:J23"/>
+    <mergeCell ref="D20:G21"/>
+    <mergeCell ref="G48:H49"/>
+    <mergeCell ref="D14:G15"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E40:G41"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="L26:Q27"/>
+    <mergeCell ref="D8:G9"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="I48:K49"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="K24:N25"/>
+    <mergeCell ref="D22:G23"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="M18:Q19"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="K12:Q13"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="D10:Q11"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="K14:Q15"/>
     <mergeCell ref="K40:L41"/>
     <mergeCell ref="M28:N29"/>
     <mergeCell ref="J26:K27"/>
@@ -3626,90 +4663,6 @@
     <mergeCell ref="E38:G39"/>
     <mergeCell ref="P44:Q45"/>
     <mergeCell ref="D44:F46"/>
-    <mergeCell ref="H8:J9"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="M18:Q19"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="K12:Q13"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="D10:Q11"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="K14:Q15"/>
-    <mergeCell ref="B2:E6"/>
-    <mergeCell ref="H22:J23"/>
-    <mergeCell ref="D20:G21"/>
-    <mergeCell ref="G48:H49"/>
-    <mergeCell ref="D14:G15"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E40:G41"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="L26:Q27"/>
-    <mergeCell ref="D8:G9"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="P22:Q23"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="Q32:Q33"/>
-    <mergeCell ref="I48:K49"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="K24:N25"/>
-    <mergeCell ref="D22:G23"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="B51:Q52"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="H12:J13"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="B35:Q36"/>
-    <mergeCell ref="B54:Q59"/>
-    <mergeCell ref="H14:J15"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P48:Q49"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K22:N23"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="H38:J39"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D24:G25"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="H40:J41"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="P20:Q21"/>
-    <mergeCell ref="E28:G29"/>
-    <mergeCell ref="I32:J33"/>
-    <mergeCell ref="M40:Q41"/>
-    <mergeCell ref="H20:J21"/>
-    <mergeCell ref="D47:F49"/>
-    <mergeCell ref="K42:L43"/>
-    <mergeCell ref="K28:L29"/>
-    <mergeCell ref="P24:Q25"/>
-    <mergeCell ref="F2:Q6"/>
-    <mergeCell ref="B32:C33"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="M38:Q39"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="H32:H33"/>
-    <mergeCell ref="K8:Q9"/>
-    <mergeCell ref="B26:C27"/>
-    <mergeCell ref="D42:J43"/>
-    <mergeCell ref="B18:C19"/>
-    <mergeCell ref="I30:J31"/>
-    <mergeCell ref="K30:L31"/>
-    <mergeCell ref="B8:C9"/>
-    <mergeCell ref="L46:O47"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="Q28:Q29"/>
-    <mergeCell ref="J18:L19"/>
-    <mergeCell ref="L48:O49"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
mudando layout da tela
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C7B9300-BA61-469E-ACD4-DBF1BB37654E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2724D6DA-41F2-4CDF-B75D-4DC532A72BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programacao" sheetId="1" r:id="rId1"/>
@@ -1007,47 +1007,28 @@
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1057,25 +1038,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1434,7 +1434,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
@@ -1444,7 +1444,7 @@
     <col min="2" max="2" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2092,7 +2092,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD23"/>
     </sheetView>
   </sheetViews>
@@ -2104,8 +2104,8 @@
     <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
@@ -3423,1138 +3423,1222 @@
   <sheetData>
     <row r="1" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="21"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="32" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="14" t="s">
         <v>189</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="23"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="16"/>
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B3" s="24"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="25"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="18"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="25"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="18"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B5" s="24"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="25"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="18"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="28"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="21"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="34" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="9" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="35" t="s">
+      <c r="I8" s="3"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="4"/>
       <c r="D10" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="7"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="4"/>
       <c r="D12" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="4"/>
       <c r="H12" s="13"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
       <c r="K12" s="13"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="4"/>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="8"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="27" t="s">
         <v>194</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="9" t="s">
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="I14" s="7"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4"/>
       <c r="K14" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="4"/>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="4"/>
       <c r="D16" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
-      <c r="Q17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="4"/>
       <c r="D18" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="9" t="s">
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="4"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="4"/>
       <c r="D20" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="15" t="s">
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="4"/>
       <c r="K20" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="3"/>
-      <c r="O20" s="17" t="s">
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="27" t="s">
         <v>201</v>
       </c>
       <c r="P20" s="13">
         <v>31200</v>
       </c>
-      <c r="Q20" s="3"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B21" s="8"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="27" t="s">
         <v>202</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="4"/>
       <c r="D22" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="15" t="s">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="I22" s="7"/>
-      <c r="J22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4"/>
       <c r="K22" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="3"/>
-      <c r="O22" s="17" t="s">
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="27" t="s">
         <v>205</v>
       </c>
       <c r="P22" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="Q22" s="3"/>
+      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B23" s="8"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="4"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="14"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="27" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="15" t="s">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="4"/>
       <c r="K24" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="3"/>
-      <c r="O24" s="17" t="s">
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="27" t="s">
         <v>208</v>
       </c>
       <c r="P24" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="Q24" s="3"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="8"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="14"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="4"/>
       <c r="D26" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="9" t="s">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K26" s="3"/>
-      <c r="L26" s="30" t="s">
+      <c r="K26" s="4"/>
+      <c r="L26" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="2:17" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="8"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="4"/>
       <c r="D28" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="4"/>
       <c r="H28" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="J28" s="3"/>
+      <c r="J28" s="4"/>
       <c r="K28" s="13">
         <v>31200</v>
       </c>
-      <c r="L28" s="3"/>
-      <c r="M28" s="6" t="s">
+      <c r="L28" s="4"/>
+      <c r="M28" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="N28" s="7"/>
+      <c r="N28" s="3"/>
       <c r="O28" s="13">
         <v>26</v>
       </c>
-      <c r="P28" s="16" t="s">
+      <c r="P28" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="Q28" s="33"/>
+      <c r="Q28" s="25"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="8"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="4"/>
-      <c r="O29" s="14"/>
-      <c r="P29" s="14"/>
-      <c r="Q29" s="14"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
+      <c r="Q29" s="23"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C30" s="3"/>
+      <c r="C30" s="4"/>
       <c r="D30" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="4"/>
       <c r="H30" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="J30" s="3"/>
+      <c r="J30" s="4"/>
       <c r="K30" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L30" s="3"/>
-      <c r="M30" s="6" t="s">
+      <c r="L30" s="4"/>
+      <c r="M30" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="N30" s="7"/>
+      <c r="N30" s="3"/>
       <c r="O30" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="P30" s="16" t="s">
+      <c r="P30" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="Q30" s="33"/>
+      <c r="Q30" s="25"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B31" s="8"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="14"/>
-      <c r="P31" s="14"/>
-      <c r="Q31" s="14"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
+      <c r="Q31" s="23"/>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="4"/>
       <c r="D32" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="4"/>
       <c r="H32" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="J32" s="3"/>
+      <c r="J32" s="4"/>
       <c r="K32" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="6" t="s">
+      <c r="L32" s="4"/>
+      <c r="M32" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="N32" s="7"/>
+      <c r="N32" s="3"/>
       <c r="O32" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="P32" s="16" t="s">
+      <c r="P32" s="29" t="s">
         <v>214</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B33" s="8"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="8"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="14"/>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="32" t="s">
+      <c r="B35" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
-      <c r="O35" s="22"/>
-      <c r="P35" s="22"/>
-      <c r="Q35" s="23"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="15"/>
+      <c r="P35" s="15"/>
+      <c r="Q35" s="16"/>
     </row>
     <row r="36" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="26"/>
-      <c r="C36" s="27"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="27"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="28"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="20"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="20"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="20"/>
+      <c r="N36" s="20"/>
+      <c r="O36" s="20"/>
+      <c r="P36" s="20"/>
+      <c r="Q36" s="21"/>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="4"/>
       <c r="D38" s="13"/>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="4"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="15" t="s">
+      <c r="I38" s="3"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="L38" s="3"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="3"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="4"/>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B39" s="8"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C40" s="3"/>
+      <c r="C40" s="4"/>
       <c r="D40" s="13"/>
-      <c r="E40" s="29" t="s">
+      <c r="E40" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="2" t="s">
+      <c r="F40" s="3"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="L40" s="3"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="7"/>
-      <c r="Q40" s="3"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="4"/>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B41" s="8"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="4"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
-      <c r="Q41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="C42" s="3"/>
+      <c r="C42" s="4"/>
       <c r="D42" s="13"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="15" t="s">
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="L42" s="3"/>
+      <c r="L42" s="4"/>
       <c r="M42" s="13"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="4"/>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B43" s="8"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="8"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="35" t="s">
         <v>224</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="19" t="s">
+      <c r="C44" s="4"/>
+      <c r="D44" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="18" t="s">
+      <c r="E44" s="3"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H44" s="3"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="15" t="s">
+      <c r="H44" s="4"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="2"/>
+      <c r="Q44" s="4"/>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B45" s="11"/>
+      <c r="B45" s="10"/>
       <c r="C45" s="12"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="20"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="11"/>
       <c r="F45" s="12"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="4"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="8"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="5"/>
-      <c r="P45" s="8"/>
-      <c r="Q45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B46" s="11"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="12"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="18" t="s">
+      <c r="D46" s="5"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H46" s="3"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="15" t="s">
+      <c r="H46" s="4"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="M46" s="7"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="4"/>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B47" s="11"/>
+      <c r="B47" s="10"/>
       <c r="C47" s="12"/>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="8"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="5"/>
-      <c r="P47" s="8"/>
-      <c r="Q47" s="5"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="7"/>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B48" s="11"/>
+      <c r="B48" s="10"/>
       <c r="C48" s="12"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="20"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="11"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="H48" s="3"/>
-      <c r="I48" s="9"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="15" t="s">
+      <c r="H48" s="4"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="M48" s="7"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="9"/>
-      <c r="Q48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="4"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B49" s="8"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="8"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="5"/>
-      <c r="P49" s="8"/>
-      <c r="Q49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="5"/>
+      <c r="Q49" s="7"/>
     </row>
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="C51" s="22"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="22"/>
-      <c r="M51" s="22"/>
-      <c r="N51" s="22"/>
-      <c r="O51" s="22"/>
-      <c r="P51" s="22"/>
-      <c r="Q51" s="23"/>
+      <c r="C51" s="15"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="15"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="15"/>
+      <c r="H51" s="15"/>
+      <c r="I51" s="15"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="16"/>
     </row>
     <row r="52" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="26"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="27"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="27"/>
-      <c r="Q52" s="28"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="20"/>
+      <c r="Q52" s="21"/>
     </row>
     <row r="53" spans="2:17" ht="7.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="54" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B54" s="13"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-      <c r="I54" s="7"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="4"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B55" s="11"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="20"/>
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="20"/>
-      <c r="I55" s="20"/>
-      <c r="J55" s="20"/>
-      <c r="K55" s="20"/>
-      <c r="L55" s="20"/>
-      <c r="M55" s="20"/>
-      <c r="N55" s="20"/>
-      <c r="O55" s="20"/>
-      <c r="P55" s="20"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
       <c r="Q55" s="12"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B56" s="11"/>
-      <c r="C56" s="20"/>
-      <c r="D56" s="20"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
-      <c r="I56" s="20"/>
-      <c r="J56" s="20"/>
-      <c r="K56" s="20"/>
-      <c r="L56" s="20"/>
-      <c r="M56" s="20"/>
-      <c r="N56" s="20"/>
-      <c r="O56" s="20"/>
-      <c r="P56" s="20"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
       <c r="Q56" s="12"/>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B57" s="11"/>
-      <c r="C57" s="20"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="20"/>
-      <c r="J57" s="20"/>
-      <c r="K57" s="20"/>
-      <c r="L57" s="20"/>
-      <c r="M57" s="20"/>
-      <c r="N57" s="20"/>
-      <c r="O57" s="20"/>
-      <c r="P57" s="20"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
       <c r="Q57" s="12"/>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B58" s="11"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="20"/>
-      <c r="I58" s="20"/>
-      <c r="J58" s="20"/>
-      <c r="K58" s="20"/>
-      <c r="L58" s="20"/>
-      <c r="M58" s="20"/>
-      <c r="N58" s="20"/>
-      <c r="O58" s="20"/>
-      <c r="P58" s="20"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
       <c r="Q58" s="12"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B59" s="8"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="6"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="6"/>
+      <c r="Q59" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="M28:N29"/>
+    <mergeCell ref="J26:K27"/>
+    <mergeCell ref="B44:C49"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="I46:K47"/>
+    <mergeCell ref="M42:Q43"/>
+    <mergeCell ref="B30:C31"/>
+    <mergeCell ref="D12:G13"/>
+    <mergeCell ref="L44:O45"/>
+    <mergeCell ref="P32:P33"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="P46:Q47"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="K20:N21"/>
+    <mergeCell ref="H24:J25"/>
+    <mergeCell ref="I44:K45"/>
+    <mergeCell ref="D16:Q17"/>
+    <mergeCell ref="G46:H47"/>
+    <mergeCell ref="E38:G39"/>
+    <mergeCell ref="P44:Q45"/>
+    <mergeCell ref="D44:F46"/>
+    <mergeCell ref="H8:J9"/>
+    <mergeCell ref="D26:I27"/>
+    <mergeCell ref="O30:O31"/>
+    <mergeCell ref="M32:N33"/>
+    <mergeCell ref="O32:O33"/>
+    <mergeCell ref="M18:Q19"/>
+    <mergeCell ref="B20:C21"/>
+    <mergeCell ref="K12:Q13"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="D10:Q11"/>
+    <mergeCell ref="B22:C23"/>
+    <mergeCell ref="K14:Q15"/>
+    <mergeCell ref="B2:E6"/>
+    <mergeCell ref="H22:J23"/>
+    <mergeCell ref="D20:G21"/>
+    <mergeCell ref="G48:H49"/>
+    <mergeCell ref="D14:G15"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E40:G41"/>
+    <mergeCell ref="P30:P31"/>
+    <mergeCell ref="L26:Q27"/>
+    <mergeCell ref="D8:G9"/>
+    <mergeCell ref="K32:L33"/>
+    <mergeCell ref="P22:Q23"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="E30:G31"/>
+    <mergeCell ref="D18:I19"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="E32:G33"/>
+    <mergeCell ref="Q32:Q33"/>
+    <mergeCell ref="I48:K49"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="K24:N25"/>
+    <mergeCell ref="D22:G23"/>
+    <mergeCell ref="B28:C29"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="B51:Q52"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="H12:J13"/>
+    <mergeCell ref="I28:J29"/>
+    <mergeCell ref="B35:Q36"/>
+    <mergeCell ref="B54:Q59"/>
+    <mergeCell ref="H14:J15"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="B24:C25"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P48:Q49"/>
+    <mergeCell ref="M30:N31"/>
+    <mergeCell ref="K22:N23"/>
+    <mergeCell ref="B40:C41"/>
+    <mergeCell ref="K38:L39"/>
+    <mergeCell ref="H38:J39"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="D24:G25"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="H40:J41"/>
+    <mergeCell ref="Q30:Q31"/>
+    <mergeCell ref="P20:Q21"/>
+    <mergeCell ref="E28:G29"/>
+    <mergeCell ref="I32:J33"/>
     <mergeCell ref="M40:Q41"/>
     <mergeCell ref="H20:J21"/>
     <mergeCell ref="D47:F49"/>
@@ -4579,90 +4663,6 @@
     <mergeCell ref="Q28:Q29"/>
     <mergeCell ref="J18:L19"/>
     <mergeCell ref="L48:O49"/>
-    <mergeCell ref="B51:Q52"/>
-    <mergeCell ref="B38:C39"/>
-    <mergeCell ref="H12:J13"/>
-    <mergeCell ref="I28:J29"/>
-    <mergeCell ref="B35:Q36"/>
-    <mergeCell ref="B54:Q59"/>
-    <mergeCell ref="H14:J15"/>
-    <mergeCell ref="B10:C11"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P48:Q49"/>
-    <mergeCell ref="M30:N31"/>
-    <mergeCell ref="K22:N23"/>
-    <mergeCell ref="B40:C41"/>
-    <mergeCell ref="K38:L39"/>
-    <mergeCell ref="H38:J39"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D24:G25"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="H40:J41"/>
-    <mergeCell ref="Q30:Q31"/>
-    <mergeCell ref="P20:Q21"/>
-    <mergeCell ref="E28:G29"/>
-    <mergeCell ref="I32:J33"/>
-    <mergeCell ref="B2:E6"/>
-    <mergeCell ref="H22:J23"/>
-    <mergeCell ref="D20:G21"/>
-    <mergeCell ref="G48:H49"/>
-    <mergeCell ref="D14:G15"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E40:G41"/>
-    <mergeCell ref="P30:P31"/>
-    <mergeCell ref="L26:Q27"/>
-    <mergeCell ref="D8:G9"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="P22:Q23"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="E30:G31"/>
-    <mergeCell ref="D18:I19"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="E32:G33"/>
-    <mergeCell ref="Q32:Q33"/>
-    <mergeCell ref="I48:K49"/>
-    <mergeCell ref="B14:C15"/>
-    <mergeCell ref="K24:N25"/>
-    <mergeCell ref="D22:G23"/>
-    <mergeCell ref="B28:C29"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="H8:J9"/>
-    <mergeCell ref="D26:I27"/>
-    <mergeCell ref="O30:O31"/>
-    <mergeCell ref="M32:N33"/>
-    <mergeCell ref="O32:O33"/>
-    <mergeCell ref="M18:Q19"/>
-    <mergeCell ref="B20:C21"/>
-    <mergeCell ref="K12:Q13"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="D10:Q11"/>
-    <mergeCell ref="B22:C23"/>
-    <mergeCell ref="K14:Q15"/>
-    <mergeCell ref="K40:L41"/>
-    <mergeCell ref="M28:N29"/>
-    <mergeCell ref="J26:K27"/>
-    <mergeCell ref="B44:C49"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="I46:K47"/>
-    <mergeCell ref="M42:Q43"/>
-    <mergeCell ref="B30:C31"/>
-    <mergeCell ref="D12:G13"/>
-    <mergeCell ref="L44:O45"/>
-    <mergeCell ref="P32:P33"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="P46:Q47"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="K20:N21"/>
-    <mergeCell ref="H24:J25"/>
-    <mergeCell ref="I44:K45"/>
-    <mergeCell ref="D16:Q17"/>
-    <mergeCell ref="G46:H47"/>
-    <mergeCell ref="E38:G39"/>
-    <mergeCell ref="P44:Q45"/>
-    <mergeCell ref="D44:F46"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
v1.5 implementação de uma rotina para limpars as areas de entrada de informação
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leitor XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2724D6DA-41F2-4CDF-B75D-4DC532A72BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E970E25-8AB9-4A34-B95C-5742A26DF601}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="241">
   <si>
     <t>Data de Entrada</t>
   </si>
@@ -384,6 +384,24 @@
     <t>LANCHOTE TRANSPORTES</t>
   </si>
   <si>
+    <t>14:46</t>
+  </si>
+  <si>
+    <t>JOAO RAMOS DE OLIVEIRA NETO</t>
+  </si>
+  <si>
+    <t>(84)991067575</t>
+  </si>
+  <si>
+    <t>355867</t>
+  </si>
+  <si>
+    <t>RXQ9H93</t>
+  </si>
+  <si>
+    <t>MONTE SERENO</t>
+  </si>
+  <si>
     <t>Movimento</t>
   </si>
   <si>
@@ -591,6 +609,21 @@
     <t>360</t>
   </si>
   <si>
+    <t>355866</t>
+  </si>
+  <si>
+    <t>564303725</t>
+  </si>
+  <si>
+    <t>355869</t>
+  </si>
+  <si>
+    <t>355868</t>
+  </si>
+  <si>
+    <t>564302825</t>
+  </si>
+  <si>
     <t>DESCARGA DE SAL</t>
   </si>
   <si>
@@ -633,16 +666,16 @@
     <t>NF 2 FORNECEDOR:</t>
   </si>
   <si>
+    <t>NF 2 PALETE:</t>
+  </si>
+  <si>
+    <t>PESO NF 2:</t>
+  </si>
+  <si>
+    <t>NF 3 FORNECEDOR:</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>NF 2 PALETE:</t>
-  </si>
-  <si>
-    <t>PESO NF 2:</t>
-  </si>
-  <si>
-    <t>NF 3 FORNECEDOR:</t>
   </si>
   <si>
     <t>NF 3 PALETE:</t>
@@ -1432,7 +1465,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
@@ -2083,6 +2116,41 @@
         <v>119</v>
       </c>
     </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" t="s">
+        <v>121</v>
+      </c>
+      <c r="D19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E19" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>5400</v>
+      </c>
+      <c r="H19" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2090,7 +2158,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A22" sqref="A22:XFD23"/>
@@ -2115,10 +2183,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2130,36 +2198,36 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="J1" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="K1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="L1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="M1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="N1" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2174,10 +2242,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G2" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -2186,16 +2254,16 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="M2" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N2">
         <v>28000</v>
@@ -2203,7 +2271,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2218,10 +2286,10 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G3" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2230,16 +2298,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M3" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N3">
         <v>27000</v>
@@ -2247,7 +2315,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2262,10 +2330,10 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2274,16 +2342,16 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="M4" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N4">
         <v>6750</v>
@@ -2291,7 +2359,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2306,28 +2374,28 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G5" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="J5" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M5" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N5">
         <v>20250</v>
@@ -2335,7 +2403,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -2362,16 +2430,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="M6" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="N6">
         <v>4200</v>
@@ -2379,7 +2447,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -2406,16 +2474,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="K7">
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="M7" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="N7">
         <v>28000</v>
@@ -2423,7 +2491,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2438,10 +2506,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2450,16 +2518,16 @@
         <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="M8" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N8">
         <v>2700</v>
@@ -2467,7 +2535,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2482,28 +2550,28 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="J9" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="K9">
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="M9" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N9">
         <v>22950</v>
@@ -2511,7 +2579,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -2526,10 +2594,10 @@
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -2538,16 +2606,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="K10">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="M10" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N10">
         <v>16200</v>
@@ -2555,7 +2623,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -2570,28 +2638,28 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G11" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="J11" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="K11">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="M11" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N11">
         <v>32400</v>
@@ -2599,7 +2667,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -2614,10 +2682,10 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -2626,16 +2694,16 @@
         <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="K12">
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="M12" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N12">
         <v>5400</v>
@@ -2643,7 +2711,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -2658,28 +2726,28 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G13" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="J13" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="M13" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N13">
         <v>24300</v>
@@ -2687,7 +2755,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -2702,10 +2770,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
@@ -2714,16 +2782,16 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="M14" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N14">
         <v>25650</v>
@@ -2731,7 +2799,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -2746,10 +2814,10 @@
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G15" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
@@ -2758,16 +2826,16 @@
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="M15" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N15">
         <v>25650</v>
@@ -2775,7 +2843,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -2790,10 +2858,10 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G16" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
@@ -2802,16 +2870,16 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>166</v>
+        <v>172</v>
       </c>
       <c r="M16" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="N16">
         <v>1350</v>
@@ -2819,7 +2887,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -2834,28 +2902,28 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="J17" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>152</v>
+        <v>158</v>
       </c>
       <c r="M17" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="N17">
         <v>28350</v>
@@ -2863,7 +2931,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -2878,10 +2946,10 @@
         <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G18" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -2890,16 +2958,16 @@
         <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="K18">
         <v>13</v>
       </c>
       <c r="L18" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="M18" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N18">
         <v>18200</v>
@@ -2907,7 +2975,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -2922,10 +2990,10 @@
         <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G19" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -2934,16 +3002,16 @@
         <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="K19">
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="M19" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N19">
         <v>9800</v>
@@ -2951,7 +3019,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -2966,10 +3034,10 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G20" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
@@ -2978,16 +3046,16 @@
         <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="M20" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N20">
         <v>6750</v>
@@ -2995,7 +3063,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -3010,28 +3078,28 @@
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G21" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H21" t="s">
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="J21" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K21">
         <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="M21" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N21">
         <v>20250</v>
@@ -3039,7 +3107,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
@@ -3054,10 +3122,10 @@
         <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G22" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -3066,16 +3134,16 @@
         <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="K22">
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="M22" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N22">
         <v>14850</v>
@@ -3083,7 +3151,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
@@ -3098,28 +3166,28 @@
         <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G23" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="J23" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="K23">
         <v>8</v>
       </c>
       <c r="L23" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="M23" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N23">
         <v>10800</v>
@@ -3127,7 +3195,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -3142,10 +3210,10 @@
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G24" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H24" t="s">
         <v>26</v>
@@ -3154,16 +3222,16 @@
         <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="K24">
         <v>11</v>
       </c>
       <c r="L24" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="M24" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N24">
         <v>14850</v>
@@ -3171,7 +3239,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -3186,28 +3254,28 @@
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="G25" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H25" t="s">
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="J25" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="K25">
         <v>8</v>
       </c>
       <c r="L25" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
       <c r="M25" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N25">
         <v>10800</v>
@@ -3215,7 +3283,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
@@ -3230,10 +3298,10 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G26" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H26" t="s">
         <v>26</v>
@@ -3242,16 +3310,16 @@
         <v>103</v>
       </c>
       <c r="J26" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="K26">
         <v>17</v>
       </c>
       <c r="L26" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="M26" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N26">
         <v>22950</v>
@@ -3259,7 +3327,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
@@ -3274,28 +3342,28 @@
         <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="G27" t="s">
-        <v>132</v>
+        <v>138</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="J27" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="K27">
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="M27" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="N27">
         <v>2700</v>
@@ -3303,7 +3371,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
@@ -3318,10 +3386,10 @@
         <v>113</v>
       </c>
       <c r="F28" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G28" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H28" t="s">
         <v>109</v>
@@ -3330,16 +3398,16 @@
         <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="K28">
         <v>28</v>
       </c>
       <c r="L28" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="M28" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="N28">
         <v>33600</v>
@@ -3347,7 +3415,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
@@ -3362,10 +3430,10 @@
         <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G29" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="H29" t="s">
         <v>109</v>
@@ -3374,19 +3442,107 @@
         <v>117</v>
       </c>
       <c r="J29" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="K29">
         <v>26</v>
       </c>
       <c r="L29" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="M29" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="N29">
         <v>31200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>136</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>124</v>
+      </c>
+      <c r="D30" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" t="s">
+        <v>125</v>
+      </c>
+      <c r="F30" t="s">
+        <v>137</v>
+      </c>
+      <c r="G30" t="s">
+        <v>138</v>
+      </c>
+      <c r="H30" t="s">
+        <v>26</v>
+      </c>
+      <c r="I30" t="s">
+        <v>123</v>
+      </c>
+      <c r="J30" t="s">
+        <v>195</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30" t="s">
+        <v>196</v>
+      </c>
+      <c r="M30" t="s">
+        <v>141</v>
+      </c>
+      <c r="N30">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" t="s">
+        <v>138</v>
+      </c>
+      <c r="H31" t="s">
+        <v>26</v>
+      </c>
+      <c r="I31" t="s">
+        <v>197</v>
+      </c>
+      <c r="J31" t="s">
+        <v>198</v>
+      </c>
+      <c r="K31">
+        <v>18</v>
+      </c>
+      <c r="L31" t="s">
+        <v>199</v>
+      </c>
+      <c r="M31" t="s">
+        <v>141</v>
+      </c>
+      <c r="N31">
+        <v>24300</v>
       </c>
     </row>
   </sheetData>
@@ -3428,7 +3584,7 @@
       <c r="D2" s="15"/>
       <c r="E2" s="16"/>
       <c r="F2" s="14" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
@@ -3516,7 +3672,7 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="33" t="s">
@@ -3526,12 +3682,12 @@
       <c r="F8" s="3"/>
       <c r="G8" s="4"/>
       <c r="H8" s="2" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="4"/>
       <c r="K8" s="24" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -3560,11 +3716,11 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="13" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -3600,11 +3756,11 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="13" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -3640,22 +3796,22 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="13" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="4"/>
       <c r="K14" s="13" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
@@ -3684,11 +3840,11 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="13" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -3724,11 +3880,11 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="13" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -3736,12 +3892,12 @@
       <c r="H18" s="3"/>
       <c r="I18" s="4"/>
       <c r="J18" s="2" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="4"/>
       <c r="M18" s="13" t="s">
-        <v>183</v>
+        <v>138</v>
       </c>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
@@ -3768,31 +3924,31 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="27" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="13" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="8" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="4"/>
       <c r="K20" s="13" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="4"/>
       <c r="O20" s="27" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="P20" s="13">
-        <v>31200</v>
+        <v>5400</v>
       </c>
       <c r="Q20" s="4"/>
     </row>
@@ -3816,31 +3972,31 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="27" t="s">
-        <v>202</v>
+        <v>213</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="13" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="8" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="4"/>
       <c r="K22" s="13" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="4"/>
       <c r="O22" s="27" t="s">
-        <v>205</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>203</v>
+        <v>215</v>
+      </c>
+      <c r="P22" s="13">
+        <v>24300</v>
       </c>
       <c r="Q22" s="4"/>
     </row>
@@ -3864,31 +4020,31 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="27" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="8" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="I24" s="3"/>
       <c r="J24" s="4"/>
       <c r="K24" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="4"/>
       <c r="O24" s="27" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="Q24" s="4"/>
     </row>
@@ -3912,11 +4068,11 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="13" t="s">
-        <v>182</v>
+        <v>137</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -3924,11 +4080,11 @@
       <c r="H26" s="3"/>
       <c r="I26" s="4"/>
       <c r="J26" s="2" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="32" t="s">
-        <v>186</v>
+        <v>141</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -3956,11 +4112,11 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="13" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E28" s="8" t="s">
         <v>4</v>
@@ -3968,25 +4124,25 @@
       <c r="F28" s="3"/>
       <c r="G28" s="4"/>
       <c r="H28" s="13" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="13">
-        <v>31200</v>
+        <v>5400</v>
       </c>
       <c r="L28" s="4"/>
       <c r="M28" s="28" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="13">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="P28" s="29" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="Q28" s="25"/>
     </row>
@@ -4010,11 +4166,11 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="13" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>4</v>
@@ -4022,25 +4178,25 @@
       <c r="F30" s="3"/>
       <c r="G30" s="4"/>
       <c r="H30" s="13" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="J30" s="4"/>
-      <c r="K30" s="13" t="s">
-        <v>203</v>
+      <c r="K30" s="13">
+        <v>24300</v>
       </c>
       <c r="L30" s="4"/>
       <c r="M30" s="28" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="N30" s="3"/>
-      <c r="O30" s="13" t="s">
-        <v>203</v>
+      <c r="O30" s="13">
+        <v>18</v>
       </c>
       <c r="P30" s="29" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="Q30" s="25"/>
     </row>
@@ -4064,11 +4220,11 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="8" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
       <c r="C32" s="4"/>
       <c r="D32" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>4</v>
@@ -4076,25 +4232,25 @@
       <c r="F32" s="3"/>
       <c r="G32" s="4"/>
       <c r="H32" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="L32" s="4"/>
       <c r="M32" s="28" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="N32" s="3"/>
       <c r="O32" s="13" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="P32" s="29" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
@@ -4119,7 +4275,7 @@
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="14" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -4157,12 +4313,12 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="8" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="13"/>
       <c r="E38" s="8" t="s">
-        <v>217</v>
+        <v>228</v>
       </c>
       <c r="F38" s="3"/>
       <c r="G38" s="4"/>
@@ -4170,7 +4326,7 @@
       <c r="I38" s="3"/>
       <c r="J38" s="4"/>
       <c r="K38" s="8" t="s">
-        <v>218</v>
+        <v>229</v>
       </c>
       <c r="L38" s="4"/>
       <c r="M38" s="2"/>
@@ -4199,12 +4355,12 @@
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="8" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
       <c r="C40" s="4"/>
       <c r="D40" s="13"/>
       <c r="E40" s="31" t="s">
-        <v>220</v>
+        <v>231</v>
       </c>
       <c r="F40" s="3"/>
       <c r="G40" s="4"/>
@@ -4212,7 +4368,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="4"/>
       <c r="K40" s="34" t="s">
-        <v>221</v>
+        <v>232</v>
       </c>
       <c r="L40" s="4"/>
       <c r="M40" s="2"/>
@@ -4241,7 +4397,7 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="8" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="13"/>
@@ -4252,7 +4408,7 @@
       <c r="I42" s="3"/>
       <c r="J42" s="4"/>
       <c r="K42" s="8" t="s">
-        <v>223</v>
+        <v>234</v>
       </c>
       <c r="L42" s="4"/>
       <c r="M42" s="13"/>
@@ -4281,23 +4437,23 @@
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="35" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="9" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="E44" s="3"/>
       <c r="F44" s="4"/>
       <c r="G44" s="22" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="2"/>
       <c r="J44" s="3"/>
       <c r="K44" s="4"/>
       <c r="L44" s="8" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
@@ -4330,14 +4486,14 @@
       <c r="E46" s="6"/>
       <c r="F46" s="7"/>
       <c r="G46" s="22" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="H46" s="4"/>
       <c r="I46" s="2"/>
       <c r="J46" s="3"/>
       <c r="K46" s="4"/>
       <c r="L46" s="8" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
@@ -4349,7 +4505,7 @@
       <c r="B47" s="10"/>
       <c r="C47" s="12"/>
       <c r="D47" s="9" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="4"/>
@@ -4372,14 +4528,14 @@
       <c r="E48" s="11"/>
       <c r="F48" s="12"/>
       <c r="G48" s="22" t="s">
-        <v>226</v>
+        <v>237</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="2"/>
       <c r="J48" s="3"/>
       <c r="K48" s="4"/>
       <c r="L48" s="8" t="s">
-        <v>227</v>
+        <v>238</v>
       </c>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -4408,7 +4564,7 @@
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B51" s="26" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15"/>

</xml_diff>

<commit_message>
inicio de uma otimização do programa
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{286D3D03-2021-4D8A-93D0-44838CA93AAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EEFE4C-9AAD-4525-8297-3DDD94F9F469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Programacao" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="287">
   <si>
     <t>Data de Entrada</t>
   </si>
@@ -492,6 +492,12 @@
     <t>CINTIA</t>
   </si>
   <si>
+    <t>das</t>
+  </si>
+  <si>
+    <t>dsa</t>
+  </si>
+  <si>
     <t>Movimento</t>
   </si>
   <si>
@@ -799,9 +805,6 @@
   </si>
   <si>
     <t>NF 2 FORNECEDOR:</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>NF 2 PALETE:</t>
@@ -1204,6 +1207,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1211,9 +1217,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1230,9 +1233,6 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1240,6 +1240,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1602,8 +1605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2505,8 +2508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2522,16 +2525,17 @@
     <col min="9" max="9" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2543,36 +2547,36 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="J1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="M1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="N1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2587,10 +2591,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -2599,16 +2603,16 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="M2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N2">
         <v>28000</v>
@@ -2616,7 +2620,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2631,10 +2635,10 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2643,16 +2647,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N3">
         <v>27000</v>
@@ -2660,7 +2664,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2675,10 +2679,10 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G4" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2687,16 +2691,16 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M4" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N4">
         <v>6750</v>
@@ -2704,7 +2708,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2719,28 +2723,28 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G5" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M5" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N5">
         <v>20250</v>
@@ -2748,7 +2752,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -2775,16 +2779,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="M6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N6">
         <v>4200</v>
@@ -2792,7 +2796,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -2819,16 +2823,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="K7">
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="M7" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N7">
         <v>28000</v>
@@ -2836,7 +2840,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2851,10 +2855,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2863,16 +2867,16 @@
         <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="M8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N8">
         <v>2700</v>
@@ -2880,7 +2884,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2895,28 +2899,28 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="J9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="K9">
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N9">
         <v>22950</v>
@@ -2924,7 +2928,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -2939,10 +2943,10 @@
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -2951,16 +2955,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="K10">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M10" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N10">
         <v>16200</v>
@@ -2968,7 +2972,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -2983,28 +2987,28 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G11" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="J11" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="K11">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M11" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N11">
         <v>32400</v>
@@ -3012,7 +3016,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -3027,10 +3031,10 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G12" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -3039,16 +3043,16 @@
         <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="K12">
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M12" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N12">
         <v>5400</v>
@@ -3056,7 +3060,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -3071,28 +3075,28 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G13" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J13" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M13" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N13">
         <v>24300</v>
@@ -3100,7 +3104,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -3115,10 +3119,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
@@ -3127,16 +3131,16 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M14" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N14">
         <v>25650</v>
@@ -3144,7 +3148,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -3159,10 +3163,10 @@
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G15" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
@@ -3171,16 +3175,16 @@
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M15" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N15">
         <v>25650</v>
@@ -3188,7 +3192,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -3203,10 +3207,10 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G16" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
@@ -3215,16 +3219,16 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="M16" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="N16">
         <v>1350</v>
@@ -3232,7 +3236,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -3247,28 +3251,28 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G17" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="J17" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="M17" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="N17">
         <v>28350</v>
@@ -3276,7 +3280,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -3291,10 +3295,10 @@
         <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G18" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -3303,16 +3307,16 @@
         <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K18">
         <v>13</v>
       </c>
       <c r="L18" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="M18" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N18">
         <v>18200</v>
@@ -3320,7 +3324,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -3335,10 +3339,10 @@
         <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -3347,16 +3351,16 @@
         <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K19">
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="M19" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N19">
         <v>9800</v>
@@ -3364,7 +3368,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -3379,10 +3383,10 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G20" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
@@ -3391,16 +3395,16 @@
         <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="M20" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N20">
         <v>6750</v>
@@ -3408,7 +3412,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -3423,28 +3427,28 @@
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G21" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H21" t="s">
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="J21" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="K21">
         <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="M21" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N21">
         <v>20250</v>
@@ -3452,7 +3456,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
@@ -3467,10 +3471,10 @@
         <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -3479,16 +3483,16 @@
         <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K22">
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N22">
         <v>14850</v>
@@ -3496,7 +3500,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
@@ -3511,28 +3515,28 @@
         <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="J23" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="K23">
         <v>8</v>
       </c>
       <c r="L23" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N23">
         <v>10800</v>
@@ -3540,7 +3544,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -3555,10 +3559,10 @@
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H24" t="s">
         <v>26</v>
@@ -3567,16 +3571,16 @@
         <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="K24">
         <v>11</v>
       </c>
       <c r="L24" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="M24" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N24">
         <v>14850</v>
@@ -3584,7 +3588,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -3599,28 +3603,28 @@
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="G25" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H25" t="s">
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="J25" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="K25">
         <v>8</v>
       </c>
       <c r="L25" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="M25" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N25">
         <v>10800</v>
@@ -3628,7 +3632,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
@@ -3643,10 +3647,10 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G26" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H26" t="s">
         <v>26</v>
@@ -3655,16 +3659,16 @@
         <v>103</v>
       </c>
       <c r="J26" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="K26">
         <v>17</v>
       </c>
       <c r="L26" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M26" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N26">
         <v>22950</v>
@@ -3672,7 +3676,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
@@ -3687,28 +3691,28 @@
         <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G27" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="J27" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="K27">
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M27" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N27">
         <v>2700</v>
@@ -3716,7 +3720,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
@@ -3731,10 +3735,10 @@
         <v>113</v>
       </c>
       <c r="F28" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G28" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H28" t="s">
         <v>109</v>
@@ -3743,16 +3747,16 @@
         <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="K28">
         <v>28</v>
       </c>
       <c r="L28" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="M28" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="N28">
         <v>33600</v>
@@ -3760,7 +3764,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
@@ -3775,10 +3779,10 @@
         <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="G29" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H29" t="s">
         <v>109</v>
@@ -3787,16 +3791,16 @@
         <v>117</v>
       </c>
       <c r="J29" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="K29">
         <v>26</v>
       </c>
       <c r="L29" t="s">
+        <v>226</v>
+      </c>
+      <c r="M29" t="s">
         <v>224</v>
-      </c>
-      <c r="M29" t="s">
-        <v>222</v>
       </c>
       <c r="N29">
         <v>31200</v>
@@ -3804,7 +3808,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
@@ -3819,10 +3823,10 @@
         <v>125</v>
       </c>
       <c r="F30" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G30" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -3831,16 +3835,16 @@
         <v>123</v>
       </c>
       <c r="J30" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="M30" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N30">
         <v>5400</v>
@@ -3848,7 +3852,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B31" t="s">
         <v>89</v>
@@ -3863,28 +3867,28 @@
         <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G31" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J31" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="K31">
         <v>18</v>
       </c>
       <c r="L31" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="M31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N31">
         <v>24300</v>
@@ -3892,7 +3896,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -3907,10 +3911,10 @@
         <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G32" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -3919,16 +3923,16 @@
         <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="K32">
         <v>4</v>
       </c>
       <c r="L32" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="M32" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N32">
         <v>5400</v>
@@ -3936,7 +3940,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B33" t="s">
         <v>89</v>
@@ -3951,28 +3955,28 @@
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G33" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
       <c r="I33" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="J33" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="K33">
         <v>15</v>
       </c>
       <c r="L33" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M33" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N33">
         <v>20250</v>
@@ -3980,7 +3984,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B34" t="s">
         <v>128</v>
@@ -3995,10 +3999,10 @@
         <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G34" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
@@ -4007,16 +4011,16 @@
         <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K34">
         <v>19</v>
       </c>
       <c r="L34" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="M34" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N34">
         <v>25650</v>
@@ -4024,7 +4028,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B35" t="s">
         <v>128</v>
@@ -4039,10 +4043,10 @@
         <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G35" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
@@ -4051,16 +4055,16 @@
         <v>134</v>
       </c>
       <c r="J35" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="K35">
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="M35" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N35">
         <v>32400</v>
@@ -4068,7 +4072,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B36" t="s">
         <v>137</v>
@@ -4083,10 +4087,10 @@
         <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H36" t="s">
         <v>26</v>
@@ -4095,16 +4099,16 @@
         <v>140</v>
       </c>
       <c r="J36" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="K36">
         <v>15</v>
       </c>
       <c r="L36" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="M36" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N36">
         <v>20250</v>
@@ -4112,7 +4116,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
@@ -4127,28 +4131,28 @@
         <v>52</v>
       </c>
       <c r="F37" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G37" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H37" t="s">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J37" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="K37">
         <v>4</v>
       </c>
       <c r="L37" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="M37" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N37">
         <v>5400</v>
@@ -4156,7 +4160,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B38" t="s">
         <v>128</v>
@@ -4171,10 +4175,10 @@
         <v>148</v>
       </c>
       <c r="F38" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G38" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H38" t="s">
         <v>145</v>
@@ -4183,16 +4187,16 @@
         <v>144</v>
       </c>
       <c r="J38" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K38">
         <v>16</v>
       </c>
       <c r="L38" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="M38" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="N38">
         <v>19600</v>
@@ -4200,7 +4204,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B39" t="s">
         <v>128</v>
@@ -4215,10 +4219,10 @@
         <v>148</v>
       </c>
       <c r="F39" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G39" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H39" t="s">
         <v>145</v>
@@ -4227,16 +4231,16 @@
         <v>144</v>
       </c>
       <c r="J39" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K39">
         <v>8</v>
       </c>
       <c r="L39" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="M39" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="N39">
         <v>9800</v>
@@ -4244,7 +4248,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B40" t="s">
         <v>128</v>
@@ -4259,10 +4263,10 @@
         <v>155</v>
       </c>
       <c r="F40" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G40" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H40" t="s">
         <v>145</v>
@@ -4271,16 +4275,16 @@
         <v>152</v>
       </c>
       <c r="J40" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="K40">
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="M40" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N40">
         <v>28800</v>
@@ -4288,7 +4292,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -4296,7 +4300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="K22" sqref="K22:N23"/>
     </sheetView>
   </sheetViews>
@@ -4325,8 +4329,8 @@
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="33" t="s">
-        <v>245</v>
+      <c r="F2" s="32" t="s">
+        <v>247</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
@@ -4342,56 +4346,56 @@
     </row>
     <row r="3" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B3" s="24"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
       <c r="E3" s="25"/>
       <c r="F3" s="24"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="20"/>
+      <c r="P3" s="20"/>
       <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
       <c r="E4" s="25"/>
       <c r="F4" s="24"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
       <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="24"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
       <c r="E5" s="25"/>
       <c r="F5" s="24"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-      <c r="N5" s="19"/>
-      <c r="O5" s="19"/>
-      <c r="P5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
       <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4414,22 +4418,22 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="31" t="s">
-        <v>128</v>
+      <c r="D8" s="34" t="s">
+        <v>156</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="3"/>
       <c r="H8" s="9" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="3"/>
       <c r="K8" s="35" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -4458,11 +4462,11 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -4498,11 +4502,11 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="13" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -4537,23 +4541,23 @@
       <c r="Q13" s="5"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
-        <v>250</v>
+      <c r="B14" s="17" t="s">
+        <v>252</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="13" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="3"/>
       <c r="H14" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="3"/>
       <c r="K14" s="13" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -4582,11 +4586,11 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -4622,11 +4626,11 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="13" t="s">
-        <v>145</v>
+        <v>26</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -4634,12 +4638,12 @@
       <c r="H18" s="7"/>
       <c r="I18" s="3"/>
       <c r="J18" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="3"/>
       <c r="M18" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -4665,32 +4669,32 @@
       <c r="Q19" s="5"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B20" s="20" t="s">
-        <v>255</v>
+      <c r="B20" s="17" t="s">
+        <v>257</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="3"/>
       <c r="H20" s="15" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="3"/>
       <c r="K20" s="13" t="s">
-        <v>234</v>
+        <v>156</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="3"/>
-      <c r="O20" s="20" t="s">
-        <v>257</v>
+      <c r="O20" s="17" t="s">
+        <v>259</v>
       </c>
       <c r="P20" s="13">
-        <v>28800</v>
+        <v>651</v>
       </c>
       <c r="Q20" s="3"/>
     </row>
@@ -4713,32 +4717,28 @@
       <c r="Q21" s="5"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
-        <v>258</v>
+      <c r="B22" s="17" t="s">
+        <v>260</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="3"/>
       <c r="H22" s="15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="K22" s="13"/>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="3"/>
-      <c r="O22" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>259</v>
+      <c r="O22" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="P22" s="13">
+        <v>351</v>
       </c>
       <c r="Q22" s="3"/>
     </row>
@@ -4761,32 +4761,28 @@
       <c r="Q23" s="5"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
-        <v>262</v>
+      <c r="B24" s="17" t="s">
+        <v>263</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
       <c r="H24" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="K24" s="13"/>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>259</v>
+      <c r="O24" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="P24" s="13">
+        <v>315</v>
       </c>
       <c r="Q24" s="3"/>
     </row>
@@ -4810,11 +4806,11 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="13" t="s">
-        <v>243</v>
+        <v>185</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -4822,11 +4818,11 @@
       <c r="H26" s="7"/>
       <c r="I26" s="3"/>
       <c r="J26" s="9" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="30" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -4854,11 +4850,11 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="13" t="s">
-        <v>244</v>
+        <v>156</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>4</v>
@@ -4866,27 +4862,27 @@
       <c r="F28" s="7"/>
       <c r="G28" s="3"/>
       <c r="H28" s="13" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="13">
-        <v>28800</v>
+        <v>651</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="13">
-        <v>24</v>
+        <v>651</v>
       </c>
       <c r="P28" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q28" s="34"/>
+        <v>271</v>
+      </c>
+      <c r="Q28" s="33"/>
     </row>
     <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="8"/>
@@ -4908,39 +4904,35 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="D30" s="13"/>
       <c r="E30" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="H30" s="13"/>
       <c r="I30" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="13" t="s">
-        <v>259</v>
+      <c r="K30" s="13">
+        <v>351</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N30" s="7"/>
-      <c r="O30" s="13" t="s">
-        <v>259</v>
+      <c r="O30" s="13">
+        <v>3123</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q30" s="34"/>
+        <v>271</v>
+      </c>
+      <c r="Q30" s="33"/>
     </row>
     <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="8"/>
@@ -4962,37 +4954,33 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="D32" s="13"/>
       <c r="E32" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="13" t="s">
-        <v>259</v>
-      </c>
+      <c r="H32" s="13"/>
       <c r="I32" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="13" t="s">
-        <v>259</v>
+      <c r="K32" s="13">
+        <v>315</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="6" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N32" s="7"/>
-      <c r="O32" s="13" t="s">
-        <v>259</v>
+      <c r="O32" s="13">
+        <v>51</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
@@ -5016,8 +5004,8 @@
     </row>
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B35" s="33" t="s">
-        <v>271</v>
+      <c r="B35" s="32" t="s">
+        <v>272</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -5055,12 +5043,12 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="13"/>
       <c r="E38" s="15" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="3"/>
@@ -5068,7 +5056,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="3"/>
       <c r="K38" s="15" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="9"/>
@@ -5097,12 +5085,12 @@
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="13"/>
       <c r="E40" s="29" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="3"/>
@@ -5110,7 +5098,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="3"/>
       <c r="K40" s="2" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="9"/>
@@ -5139,7 +5127,7 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="13"/>
@@ -5150,7 +5138,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="3"/>
       <c r="K42" s="15" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="13"/>
@@ -5179,23 +5167,23 @@
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="18" t="s">
-        <v>281</v>
+      <c r="D44" s="19" t="s">
+        <v>282</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="17" t="s">
-        <v>282</v>
+      <c r="G44" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="9"/>
       <c r="J44" s="7"/>
       <c r="K44" s="3"/>
       <c r="L44" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
@@ -5207,7 +5195,7 @@
       <c r="B45" s="11"/>
       <c r="C45" s="12"/>
       <c r="D45" s="11"/>
-      <c r="E45" s="19"/>
+      <c r="E45" s="20"/>
       <c r="F45" s="12"/>
       <c r="G45" s="8"/>
       <c r="H45" s="5"/>
@@ -5227,15 +5215,15 @@
       <c r="D46" s="8"/>
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="17" t="s">
-        <v>282</v>
+      <c r="G46" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="9"/>
       <c r="J46" s="7"/>
       <c r="K46" s="3"/>
       <c r="L46" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
@@ -5246,8 +5234,8 @@
     <row r="47" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
-      <c r="D47" s="18" t="s">
-        <v>284</v>
+      <c r="D47" s="19" t="s">
+        <v>285</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="3"/>
@@ -5267,17 +5255,17 @@
       <c r="B48" s="11"/>
       <c r="C48" s="12"/>
       <c r="D48" s="11"/>
-      <c r="E48" s="19"/>
+      <c r="E48" s="20"/>
       <c r="F48" s="12"/>
-      <c r="G48" s="17" t="s">
-        <v>282</v>
+      <c r="G48" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="9"/>
       <c r="J48" s="7"/>
       <c r="K48" s="3"/>
       <c r="L48" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -5305,8 +5293,8 @@
     </row>
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B51" s="32" t="s">
-        <v>285</v>
+      <c r="B51" s="31" t="s">
+        <v>286</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5363,74 +5351,74 @@
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B55" s="11"/>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
-      <c r="H55" s="19"/>
-      <c r="I55" s="19"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
-      <c r="L55" s="19"/>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19"/>
-      <c r="O55" s="19"/>
-      <c r="P55" s="19"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="20"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="20"/>
+      <c r="L55" s="20"/>
+      <c r="M55" s="20"/>
+      <c r="N55" s="20"/>
+      <c r="O55" s="20"/>
+      <c r="P55" s="20"/>
       <c r="Q55" s="12"/>
     </row>
     <row r="56" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B56" s="11"/>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
-      <c r="L56" s="19"/>
-      <c r="M56" s="19"/>
-      <c r="N56" s="19"/>
-      <c r="O56" s="19"/>
-      <c r="P56" s="19"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="20"/>
+      <c r="L56" s="20"/>
+      <c r="M56" s="20"/>
+      <c r="N56" s="20"/>
+      <c r="O56" s="20"/>
+      <c r="P56" s="20"/>
       <c r="Q56" s="12"/>
     </row>
     <row r="57" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B57" s="11"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
-      <c r="I57" s="19"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
-      <c r="L57" s="19"/>
-      <c r="M57" s="19"/>
-      <c r="N57" s="19"/>
-      <c r="O57" s="19"/>
-      <c r="P57" s="19"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="20"/>
+      <c r="L57" s="20"/>
+      <c r="M57" s="20"/>
+      <c r="N57" s="20"/>
+      <c r="O57" s="20"/>
+      <c r="P57" s="20"/>
       <c r="Q57" s="12"/>
     </row>
     <row r="58" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B58" s="11"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="19"/>
-      <c r="P58" s="19"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="20"/>
+      <c r="L58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="N58" s="20"/>
+      <c r="O58" s="20"/>
+      <c r="P58" s="20"/>
       <c r="Q58" s="12"/>
     </row>
     <row r="59" spans="2:17" x14ac:dyDescent="0.3">
@@ -5562,8 +5550,8 @@
     <mergeCell ref="P44:Q45"/>
     <mergeCell ref="D44:F46"/>
   </mergeCells>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125978" footer="0.31496062992125978"/>
+  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
teste para otimização do codigo
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Leitor XML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EEFE4C-9AAD-4525-8297-3DDD94F9F469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDA256-CDB3-44D8-8DA0-8AF6EE7A684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="293">
   <si>
     <t>Data de Entrada</t>
   </si>
@@ -492,10 +492,19 @@
     <t>CINTIA</t>
   </si>
   <si>
-    <t>das</t>
-  </si>
-  <si>
-    <t>dsa</t>
+    <t>15:54</t>
+  </si>
+  <si>
+    <t>JACO PEREIRA DANTES</t>
+  </si>
+  <si>
+    <t>(84)996589874</t>
+  </si>
+  <si>
+    <t>355890</t>
+  </si>
+  <si>
+    <t>RYE3J61</t>
   </si>
   <si>
     <t>Movimento</t>
@@ -765,6 +774,12 @@
     <t>1056250124</t>
   </si>
   <si>
+    <t>355889</t>
+  </si>
+  <si>
+    <t>140303425</t>
+  </si>
+  <si>
     <t>DESCARGA DE SAL</t>
   </si>
   <si>
@@ -805,6 +820,9 @@
   </si>
   <si>
     <t>NF 2 FORNECEDOR:</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>NF 2 PALETE:</t>
@@ -1603,7 +1621,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:XFD26"/>
@@ -2499,6 +2517,41 @@
         <v>155</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" t="s">
+        <v>156</v>
+      </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
+        <v>158</v>
+      </c>
+      <c r="E26" t="s">
+        <v>159</v>
+      </c>
+      <c r="F26" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26">
+        <v>29700</v>
+      </c>
+      <c r="H26" t="s">
+        <v>160</v>
+      </c>
+      <c r="I26" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" t="s">
+        <v>19</v>
+      </c>
+      <c r="K26" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2506,7 +2559,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD41"/>
@@ -2525,17 +2578,17 @@
     <col min="9" max="9" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2547,36 +2600,36 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="J1" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="K1" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="L1" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="N1" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2591,10 +2644,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -2603,16 +2656,16 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="M2" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N2">
         <v>28000</v>
@@ -2620,7 +2673,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2635,10 +2688,10 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2647,16 +2700,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
+        <v>179</v>
+      </c>
+      <c r="M3" t="s">
         <v>176</v>
-      </c>
-      <c r="M3" t="s">
-        <v>173</v>
       </c>
       <c r="N3">
         <v>27000</v>
@@ -2664,7 +2717,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2679,10 +2732,10 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2691,16 +2744,16 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="M4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N4">
         <v>6750</v>
@@ -2708,7 +2761,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2723,28 +2776,28 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="J5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5" t="s">
+        <v>179</v>
+      </c>
+      <c r="M5" t="s">
         <v>176</v>
-      </c>
-      <c r="M5" t="s">
-        <v>173</v>
       </c>
       <c r="N5">
         <v>20250</v>
@@ -2752,7 +2805,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -2779,16 +2832,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="M6" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="N6">
         <v>4200</v>
@@ -2796,7 +2849,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -2823,16 +2876,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="K7">
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="M7" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="N7">
         <v>28000</v>
@@ -2840,7 +2893,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2855,10 +2908,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G8" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2867,16 +2920,16 @@
         <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="M8" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N8">
         <v>2700</v>
@@ -2884,7 +2937,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2899,28 +2952,28 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G9" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="J9" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="K9">
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="M9" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N9">
         <v>22950</v>
@@ -2928,7 +2981,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -2943,10 +2996,10 @@
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G10" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -2955,16 +3008,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="K10">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="M10" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N10">
         <v>16200</v>
@@ -2972,7 +3025,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -2987,28 +3040,28 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G11" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="J11" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="K11">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="M11" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N11">
         <v>32400</v>
@@ -3016,7 +3069,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -3031,10 +3084,10 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -3043,16 +3096,16 @@
         <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="K12">
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M12" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N12">
         <v>5400</v>
@@ -3060,7 +3113,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -3075,28 +3128,28 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G13" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="J13" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="M13" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N13">
         <v>24300</v>
@@ -3104,7 +3157,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -3119,10 +3172,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G14" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
@@ -3131,16 +3184,16 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="M14" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N14">
         <v>25650</v>
@@ -3148,7 +3201,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -3163,10 +3216,10 @@
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
@@ -3175,16 +3228,16 @@
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="M15" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N15">
         <v>25650</v>
@@ -3192,7 +3245,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -3207,10 +3260,10 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G16" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
@@ -3219,16 +3272,16 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="M16" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="N16">
         <v>1350</v>
@@ -3236,7 +3289,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -3251,28 +3304,28 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G17" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="J17" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="M17" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="N17">
         <v>28350</v>
@@ -3280,7 +3333,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -3295,10 +3348,10 @@
         <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -3307,16 +3360,16 @@
         <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K18">
         <v>13</v>
       </c>
       <c r="L18" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="M18" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N18">
         <v>18200</v>
@@ -3324,7 +3377,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -3339,10 +3392,10 @@
         <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G19" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -3351,16 +3404,16 @@
         <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="K19">
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="M19" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N19">
         <v>9800</v>
@@ -3368,7 +3421,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -3383,10 +3436,10 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G20" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
@@ -3395,16 +3448,16 @@
         <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="M20" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N20">
         <v>6750</v>
@@ -3412,7 +3465,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -3427,28 +3480,28 @@
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G21" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H21" t="s">
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="J21" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K21">
         <v>15</v>
       </c>
       <c r="L21" t="s">
+        <v>179</v>
+      </c>
+      <c r="M21" t="s">
         <v>176</v>
-      </c>
-      <c r="M21" t="s">
-        <v>173</v>
       </c>
       <c r="N21">
         <v>20250</v>
@@ -3456,7 +3509,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
@@ -3471,10 +3524,10 @@
         <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -3483,16 +3536,16 @@
         <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="K22">
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="M22" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N22">
         <v>14850</v>
@@ -3500,7 +3553,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
@@ -3515,28 +3568,28 @@
         <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G23" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="J23" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="K23">
         <v>8</v>
       </c>
       <c r="L23" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="M23" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N23">
         <v>10800</v>
@@ -3544,7 +3597,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -3559,10 +3612,10 @@
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G24" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H24" t="s">
         <v>26</v>
@@ -3571,16 +3624,16 @@
         <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="K24">
         <v>11</v>
       </c>
       <c r="L24" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="M24" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N24">
         <v>14850</v>
@@ -3588,7 +3641,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -3603,28 +3656,28 @@
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G25" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H25" t="s">
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="J25" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="K25">
         <v>8</v>
       </c>
       <c r="L25" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M25" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N25">
         <v>10800</v>
@@ -3632,7 +3685,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
@@ -3647,10 +3700,10 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H26" t="s">
         <v>26</v>
@@ -3659,16 +3712,16 @@
         <v>103</v>
       </c>
       <c r="J26" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="K26">
         <v>17</v>
       </c>
       <c r="L26" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="M26" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N26">
         <v>22950</v>
@@ -3676,7 +3729,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
@@ -3691,28 +3744,28 @@
         <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G27" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J27" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="K27">
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="M27" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N27">
         <v>2700</v>
@@ -3720,7 +3773,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
@@ -3735,10 +3788,10 @@
         <v>113</v>
       </c>
       <c r="F28" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G28" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H28" t="s">
         <v>109</v>
@@ -3747,16 +3800,16 @@
         <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K28">
         <v>28</v>
       </c>
       <c r="L28" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="M28" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="N28">
         <v>33600</v>
@@ -3764,7 +3817,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
@@ -3779,10 +3832,10 @@
         <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="G29" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="H29" t="s">
         <v>109</v>
@@ -3791,16 +3844,16 @@
         <v>117</v>
       </c>
       <c r="J29" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="K29">
         <v>26</v>
       </c>
       <c r="L29" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="M29" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="N29">
         <v>31200</v>
@@ -3808,7 +3861,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
@@ -3823,10 +3876,10 @@
         <v>125</v>
       </c>
       <c r="F30" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G30" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -3835,16 +3888,16 @@
         <v>123</v>
       </c>
       <c r="J30" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="M30" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N30">
         <v>5400</v>
@@ -3852,7 +3905,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B31" t="s">
         <v>89</v>
@@ -3867,28 +3920,28 @@
         <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="J31" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="K31">
         <v>18</v>
       </c>
       <c r="L31" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="M31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N31">
         <v>24300</v>
@@ -3896,7 +3949,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -3911,10 +3964,10 @@
         <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G32" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -3923,16 +3976,16 @@
         <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="K32">
         <v>4</v>
       </c>
       <c r="L32" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="M32" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N32">
         <v>5400</v>
@@ -3940,7 +3993,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B33" t="s">
         <v>89</v>
@@ -3955,28 +4008,28 @@
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G33" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
       <c r="I33" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="J33" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="K33">
         <v>15</v>
       </c>
       <c r="L33" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="M33" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N33">
         <v>20250</v>
@@ -3984,7 +4037,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B34" t="s">
         <v>128</v>
@@ -3999,10 +4052,10 @@
         <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G34" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
@@ -4011,16 +4064,16 @@
         <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K34">
         <v>19</v>
       </c>
       <c r="L34" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="M34" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N34">
         <v>25650</v>
@@ -4028,7 +4081,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
         <v>128</v>
@@ -4043,10 +4096,10 @@
         <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G35" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
@@ -4055,16 +4108,16 @@
         <v>134</v>
       </c>
       <c r="J35" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="K35">
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="M35" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N35">
         <v>32400</v>
@@ -4072,7 +4125,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B36" t="s">
         <v>137</v>
@@ -4087,10 +4140,10 @@
         <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G36" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H36" t="s">
         <v>26</v>
@@ -4099,16 +4152,16 @@
         <v>140</v>
       </c>
       <c r="J36" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="K36">
         <v>15</v>
       </c>
       <c r="L36" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="M36" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N36">
         <v>20250</v>
@@ -4116,7 +4169,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
@@ -4131,28 +4184,28 @@
         <v>52</v>
       </c>
       <c r="F37" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G37" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H37" t="s">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="J37" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K37">
         <v>4</v>
       </c>
       <c r="L37" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="M37" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N37">
         <v>5400</v>
@@ -4160,7 +4213,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B38" t="s">
         <v>128</v>
@@ -4175,10 +4228,10 @@
         <v>148</v>
       </c>
       <c r="F38" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H38" t="s">
         <v>145</v>
@@ -4187,16 +4240,16 @@
         <v>144</v>
       </c>
       <c r="J38" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K38">
         <v>16</v>
       </c>
       <c r="L38" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="M38" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="N38">
         <v>19600</v>
@@ -4204,7 +4257,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B39" t="s">
         <v>128</v>
@@ -4219,10 +4272,10 @@
         <v>148</v>
       </c>
       <c r="F39" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G39" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H39" t="s">
         <v>145</v>
@@ -4231,16 +4284,16 @@
         <v>144</v>
       </c>
       <c r="J39" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K39">
         <v>8</v>
       </c>
       <c r="L39" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="M39" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="N39">
         <v>9800</v>
@@ -4248,7 +4301,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B40" t="s">
         <v>128</v>
@@ -4263,10 +4316,10 @@
         <v>155</v>
       </c>
       <c r="F40" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H40" t="s">
         <v>145</v>
@@ -4275,19 +4328,63 @@
         <v>152</v>
       </c>
       <c r="J40" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="K40">
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="M40" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="N40">
         <v>28800</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>171</v>
+      </c>
+      <c r="B41" t="s">
+        <v>128</v>
+      </c>
+      <c r="C41" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" t="s">
+        <v>172</v>
+      </c>
+      <c r="G41" t="s">
+        <v>173</v>
+      </c>
+      <c r="H41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>159</v>
+      </c>
+      <c r="J41" t="s">
+        <v>250</v>
+      </c>
+      <c r="K41">
+        <v>22</v>
+      </c>
+      <c r="L41" t="s">
+        <v>251</v>
+      </c>
+      <c r="M41" t="s">
+        <v>186</v>
+      </c>
+      <c r="N41">
+        <v>29700</v>
       </c>
     </row>
   </sheetData>
@@ -4330,7 +4427,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="32" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
@@ -4418,17 +4515,17 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="34" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="3"/>
       <c r="H8" s="9" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="3"/>
@@ -4462,11 +4559,11 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="13" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -4502,11 +4599,11 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="13" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -4542,22 +4639,22 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="13" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="3"/>
       <c r="H14" s="9" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="3"/>
       <c r="K14" s="13" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -4586,11 +4683,11 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="13" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -4626,7 +4723,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="13" t="s">
@@ -4638,12 +4735,12 @@
       <c r="H18" s="7"/>
       <c r="I18" s="3"/>
       <c r="J18" s="9" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="3"/>
       <c r="M18" s="13" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -4670,31 +4767,31 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="17" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="3"/>
       <c r="H20" s="15" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="3"/>
       <c r="K20" s="13" t="s">
-        <v>156</v>
+        <v>250</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="3"/>
       <c r="O20" s="17" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="P20" s="13">
-        <v>651</v>
+        <v>29700</v>
       </c>
       <c r="Q20" s="3"/>
     </row>
@@ -4718,27 +4815,31 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="3"/>
       <c r="H22" s="15" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="13"/>
+      <c r="K22" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="3"/>
       <c r="O22" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="P22" s="13">
-        <v>351</v>
+        <v>268</v>
+      </c>
+      <c r="P22" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="Q22" s="3"/>
     </row>
@@ -4762,27 +4863,31 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
       <c r="H24" s="15" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="13"/>
+      <c r="K24" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="3"/>
       <c r="O24" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="P24" s="13">
-        <v>315</v>
+        <v>271</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="Q24" s="3"/>
     </row>
@@ -4806,11 +4911,11 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>266</v>
+        <v>272</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="13" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -4818,11 +4923,11 @@
       <c r="H26" s="7"/>
       <c r="I26" s="3"/>
       <c r="J26" s="9" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="30" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -4850,11 +4955,11 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="13" t="s">
-        <v>156</v>
+        <v>251</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>4</v>
@@ -4862,25 +4967,25 @@
       <c r="F28" s="7"/>
       <c r="G28" s="3"/>
       <c r="H28" s="13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="13">
-        <v>651</v>
+        <v>29700</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="6" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="13">
-        <v>651</v>
+        <v>22</v>
       </c>
       <c r="P28" s="16" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="Q28" s="33"/>
     </row>
@@ -4904,33 +5009,37 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="13"/>
+      <c r="D30" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="E30" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="13"/>
+      <c r="H30" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="I30" s="15" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="13">
-        <v>351</v>
+      <c r="K30" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="6" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="N30" s="7"/>
-      <c r="O30" s="13">
-        <v>3123</v>
+      <c r="O30" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="Q30" s="33"/>
     </row>
@@ -4954,33 +5063,37 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="13"/>
+      <c r="D32" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="E32" s="15" t="s">
         <v>4</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="3"/>
-      <c r="H32" s="13"/>
+      <c r="H32" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="I32" s="15" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="13">
-        <v>315</v>
+      <c r="K32" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="6" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="N32" s="7"/>
-      <c r="O32" s="13">
-        <v>51</v>
+      <c r="O32" s="13" t="s">
+        <v>266</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
@@ -5005,7 +5118,7 @@
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="32" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -5043,12 +5156,12 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="13"/>
       <c r="E38" s="15" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="3"/>
@@ -5056,7 +5169,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="3"/>
       <c r="K38" s="15" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="9"/>
@@ -5085,12 +5198,12 @@
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="13"/>
       <c r="E40" s="29" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="3"/>
@@ -5098,7 +5211,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="3"/>
       <c r="K40" s="2" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="9"/>
@@ -5127,7 +5240,7 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="13"/>
@@ -5138,7 +5251,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="3"/>
       <c r="K42" s="15" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="13"/>
@@ -5167,23 +5280,23 @@
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="19" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="3"/>
       <c r="G44" s="18" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="9"/>
       <c r="J44" s="7"/>
       <c r="K44" s="3"/>
       <c r="L44" s="15" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
@@ -5216,14 +5329,14 @@
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="G46" s="18" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="9"/>
       <c r="J46" s="7"/>
       <c r="K46" s="3"/>
       <c r="L46" s="15" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
@@ -5235,7 +5348,7 @@
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
       <c r="D47" s="19" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="3"/>
@@ -5258,14 +5371,14 @@
       <c r="E48" s="20"/>
       <c r="F48" s="12"/>
       <c r="G48" s="18" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="9"/>
       <c r="J48" s="7"/>
       <c r="K48" s="3"/>
       <c r="L48" s="15" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -5294,7 +5407,7 @@
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B51" s="31" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>
@@ -5551,7 +5664,7 @@
     <mergeCell ref="D44:F46"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.31496062992125978" footer="0.31496062992125978"/>
-  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inserção de novos dados na planhila dados.xlxs
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Leitor XML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FDA256-CDB3-44D8-8DA0-8AF6EE7A684B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB82BF9-57C9-4F5A-8037-C8E680A8B5E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="342">
   <si>
     <t>Data de Entrada</t>
   </si>
@@ -507,6 +507,96 @@
     <t>RYE3J61</t>
   </si>
   <si>
+    <t>05:51</t>
+  </si>
+  <si>
+    <t>VALDISMAR MARTINS DA FONSECA</t>
+  </si>
+  <si>
+    <t>(84)998090247</t>
+  </si>
+  <si>
+    <t>355905</t>
+  </si>
+  <si>
+    <t>RXR6C45</t>
+  </si>
+  <si>
+    <t>14/02/2025</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>FRANCISCO JOSE</t>
+  </si>
+  <si>
+    <t>(11)958672456</t>
+  </si>
+  <si>
+    <t>354574</t>
+  </si>
+  <si>
+    <t>08:07</t>
+  </si>
+  <si>
+    <t>ALEXSANDER DA SILVA BONIFACIO</t>
+  </si>
+  <si>
+    <t>354902</t>
+  </si>
+  <si>
+    <t>09:03</t>
+  </si>
+  <si>
+    <t>WALTER LIRA MIRANDA</t>
+  </si>
+  <si>
+    <t>(11)957288225</t>
+  </si>
+  <si>
+    <t>354811</t>
+  </si>
+  <si>
+    <t>ATF0858</t>
+  </si>
+  <si>
+    <t>13:33</t>
+  </si>
+  <si>
+    <t>MICHAEL DE JEJUS</t>
+  </si>
+  <si>
+    <t>(85)987194818</t>
+  </si>
+  <si>
+    <t>355840</t>
+  </si>
+  <si>
+    <t>GAN7418</t>
+  </si>
+  <si>
+    <t>09:38</t>
+  </si>
+  <si>
+    <t>354575</t>
+  </si>
+  <si>
+    <t>14:41</t>
+  </si>
+  <si>
+    <t>CARLOS ROBERTO TOQUERO</t>
+  </si>
+  <si>
+    <t>(11)988894997</t>
+  </si>
+  <si>
+    <t>354641</t>
+  </si>
+  <si>
+    <t>FRC3B40</t>
+  </si>
+  <si>
     <t>Movimento</t>
   </si>
   <si>
@@ -780,6 +870,63 @@
     <t>140303425</t>
   </si>
   <si>
+    <t>355904</t>
+  </si>
+  <si>
+    <t>354572</t>
+  </si>
+  <si>
+    <t>354901</t>
+  </si>
+  <si>
+    <t>354904</t>
+  </si>
+  <si>
+    <t>354903</t>
+  </si>
+  <si>
+    <t>140302025</t>
+  </si>
+  <si>
+    <t>354810</t>
+  </si>
+  <si>
+    <t>354813</t>
+  </si>
+  <si>
+    <t>354812</t>
+  </si>
+  <si>
+    <t>355839</t>
+  </si>
+  <si>
+    <t>540303625</t>
+  </si>
+  <si>
+    <t>355838</t>
+  </si>
+  <si>
+    <t>355837</t>
+  </si>
+  <si>
+    <t>354573</t>
+  </si>
+  <si>
+    <t>354577</t>
+  </si>
+  <si>
+    <t>354576</t>
+  </si>
+  <si>
+    <t>354640</t>
+  </si>
+  <si>
+    <t>354643</t>
+  </si>
+  <si>
+    <t>354642</t>
+  </si>
+  <si>
     <t>DESCARGA DE SAL</t>
   </si>
   <si>
@@ -822,16 +969,16 @@
     <t>NF 2 FORNECEDOR:</t>
   </si>
   <si>
+    <t>NF 2 PALETE:</t>
+  </si>
+  <si>
+    <t>PESO NF 2:</t>
+  </si>
+  <si>
+    <t>NF 3 FORNECEDOR:</t>
+  </si>
+  <si>
     <t/>
-  </si>
-  <si>
-    <t>NF 2 PALETE:</t>
-  </si>
-  <si>
-    <t>PESO NF 2:</t>
-  </si>
-  <si>
-    <t>NF 3 FORNECEDOR:</t>
   </si>
   <si>
     <t>NF 3 PALETE:</t>
@@ -1621,7 +1768,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:XFD26"/>
@@ -2552,6 +2699,251 @@
         <v>125</v>
       </c>
     </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" t="s">
+        <v>162</v>
+      </c>
+      <c r="D27" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27" t="s">
+        <v>164</v>
+      </c>
+      <c r="F27" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27">
+        <v>29700</v>
+      </c>
+      <c r="H27" t="s">
+        <v>165</v>
+      </c>
+      <c r="I27" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" t="s">
+        <v>170</v>
+      </c>
+      <c r="F28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28">
+        <v>25650</v>
+      </c>
+      <c r="H28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>166</v>
+      </c>
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C29" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E29" t="s">
+        <v>173</v>
+      </c>
+      <c r="F29" t="s">
+        <v>26</v>
+      </c>
+      <c r="G29">
+        <v>8100</v>
+      </c>
+      <c r="H29" t="s">
+        <v>94</v>
+      </c>
+      <c r="I29" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" t="s">
+        <v>19</v>
+      </c>
+      <c r="K29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>166</v>
+      </c>
+      <c r="B30" t="s">
+        <v>174</v>
+      </c>
+      <c r="C30" t="s">
+        <v>175</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E30" t="s">
+        <v>177</v>
+      </c>
+      <c r="F30" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30">
+        <v>9450</v>
+      </c>
+      <c r="H30" t="s">
+        <v>178</v>
+      </c>
+      <c r="I30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
+        <v>19</v>
+      </c>
+      <c r="K30" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>179</v>
+      </c>
+      <c r="C31" t="s">
+        <v>180</v>
+      </c>
+      <c r="D31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E31" t="s">
+        <v>182</v>
+      </c>
+      <c r="F31" t="s">
+        <v>26</v>
+      </c>
+      <c r="G31">
+        <v>6750</v>
+      </c>
+      <c r="H31" t="s">
+        <v>183</v>
+      </c>
+      <c r="I31" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32">
+        <v>6750</v>
+      </c>
+      <c r="H32" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" t="s">
+        <v>19</v>
+      </c>
+      <c r="K32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>166</v>
+      </c>
+      <c r="B33" t="s">
+        <v>186</v>
+      </c>
+      <c r="C33" t="s">
+        <v>187</v>
+      </c>
+      <c r="D33" t="s">
+        <v>188</v>
+      </c>
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+      <c r="F33" t="s">
+        <v>26</v>
+      </c>
+      <c r="G33">
+        <v>10800</v>
+      </c>
+      <c r="H33" t="s">
+        <v>190</v>
+      </c>
+      <c r="I33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J33" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" t="s">
+        <v>95</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2559,7 +2951,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD41"/>
@@ -2585,10 +2977,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -2600,36 +2992,36 @@
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="G1" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>165</v>
+        <v>195</v>
       </c>
       <c r="J1" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="K1" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="L1" t="s">
-        <v>168</v>
+        <v>198</v>
       </c>
       <c r="M1" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="N1" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -2644,10 +3036,10 @@
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G2" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
@@ -2656,16 +3048,16 @@
         <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>174</v>
+        <v>204</v>
       </c>
       <c r="K2">
         <v>20</v>
       </c>
       <c r="L2" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
       <c r="M2" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N2">
         <v>28000</v>
@@ -2673,7 +3065,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B3" t="s">
         <v>21</v>
@@ -2688,10 +3080,10 @@
         <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G3" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H3" t="s">
         <v>26</v>
@@ -2700,16 +3092,16 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="K3">
         <v>20</v>
       </c>
       <c r="L3" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="M3" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N3">
         <v>27000</v>
@@ -2717,7 +3109,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
@@ -2732,10 +3124,10 @@
         <v>36</v>
       </c>
       <c r="F4" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G4" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H4" t="s">
         <v>26</v>
@@ -2744,16 +3136,16 @@
         <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="M4" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N4">
         <v>6750</v>
@@ -2761,7 +3153,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -2776,28 +3168,28 @@
         <v>36</v>
       </c>
       <c r="F5" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G5" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
       </c>
       <c r="I5" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="J5" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="K5">
         <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="M5" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N5">
         <v>20250</v>
@@ -2805,7 +3197,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
@@ -2832,16 +3224,16 @@
         <v>41</v>
       </c>
       <c r="J6" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="K6">
         <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>185</v>
+        <v>215</v>
       </c>
       <c r="M6" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="N6">
         <v>4200</v>
@@ -2849,7 +3241,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B7" t="s">
         <v>37</v>
@@ -2876,16 +3268,16 @@
         <v>41</v>
       </c>
       <c r="J7" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="K7">
         <v>20</v>
       </c>
       <c r="L7" t="s">
-        <v>187</v>
+        <v>217</v>
       </c>
       <c r="M7" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="N7">
         <v>28000</v>
@@ -2893,7 +3285,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
@@ -2908,10 +3300,10 @@
         <v>52</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H8" t="s">
         <v>26</v>
@@ -2920,16 +3312,16 @@
         <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="K8">
         <v>2</v>
       </c>
       <c r="L8" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="M8" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N8">
         <v>2700</v>
@@ -2937,7 +3329,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
@@ -2952,28 +3344,28 @@
         <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G9" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H9" t="s">
         <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="J9" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="K9">
         <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="M9" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N9">
         <v>22950</v>
@@ -2981,7 +3373,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -2996,10 +3388,10 @@
         <v>59</v>
       </c>
       <c r="F10" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G10" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H10" t="s">
         <v>26</v>
@@ -3008,16 +3400,16 @@
         <v>56</v>
       </c>
       <c r="J10" t="s">
-        <v>194</v>
+        <v>224</v>
       </c>
       <c r="K10">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="M10" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N10">
         <v>16200</v>
@@ -3025,7 +3417,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -3040,28 +3432,28 @@
         <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G11" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H11" t="s">
         <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>196</v>
+        <v>226</v>
       </c>
       <c r="J11" t="s">
-        <v>197</v>
+        <v>227</v>
       </c>
       <c r="K11">
         <v>24</v>
       </c>
       <c r="L11" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="M11" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N11">
         <v>32400</v>
@@ -3069,7 +3461,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B12" t="s">
         <v>37</v>
@@ -3084,10 +3476,10 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G12" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H12" t="s">
         <v>26</v>
@@ -3096,16 +3488,16 @@
         <v>63</v>
       </c>
       <c r="J12" t="s">
-        <v>198</v>
+        <v>228</v>
       </c>
       <c r="K12">
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="M12" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N12">
         <v>5400</v>
@@ -3113,7 +3505,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s">
         <v>37</v>
@@ -3128,28 +3520,28 @@
         <v>65</v>
       </c>
       <c r="F13" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G13" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H13" t="s">
         <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="J13" t="s">
-        <v>201</v>
+        <v>231</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
       <c r="L13" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="M13" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N13">
         <v>24300</v>
@@ -3157,7 +3549,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
@@ -3172,10 +3564,10 @@
         <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G14" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H14" t="s">
         <v>26</v>
@@ -3184,16 +3576,16 @@
         <v>69</v>
       </c>
       <c r="J14" t="s">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
       <c r="L14" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="M14" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N14">
         <v>25650</v>
@@ -3201,7 +3593,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
@@ -3216,10 +3608,10 @@
         <v>52</v>
       </c>
       <c r="F15" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G15" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H15" t="s">
         <v>26</v>
@@ -3228,16 +3620,16 @@
         <v>74</v>
       </c>
       <c r="J15" t="s">
-        <v>204</v>
+        <v>234</v>
       </c>
       <c r="K15">
         <v>19</v>
       </c>
       <c r="L15" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="M15" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N15">
         <v>25650</v>
@@ -3245,7 +3637,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -3260,10 +3652,10 @@
         <v>65</v>
       </c>
       <c r="F16" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G16" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
         <v>26</v>
@@ -3272,16 +3664,16 @@
         <v>79</v>
       </c>
       <c r="J16" t="s">
-        <v>206</v>
+        <v>236</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>207</v>
+        <v>237</v>
       </c>
       <c r="M16" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="N16">
         <v>1350</v>
@@ -3289,7 +3681,7 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B17" t="s">
         <v>37</v>
@@ -3304,28 +3696,28 @@
         <v>65</v>
       </c>
       <c r="F17" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G17" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H17" t="s">
         <v>26</v>
       </c>
       <c r="I17" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="J17" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="K17">
         <v>21</v>
       </c>
       <c r="L17" t="s">
-        <v>193</v>
+        <v>223</v>
       </c>
       <c r="M17" t="s">
-        <v>208</v>
+        <v>238</v>
       </c>
       <c r="N17">
         <v>28350</v>
@@ -3333,7 +3725,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>81</v>
@@ -3348,10 +3740,10 @@
         <v>87</v>
       </c>
       <c r="F18" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G18" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -3360,16 +3752,16 @@
         <v>85</v>
       </c>
       <c r="J18" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="K18">
         <v>13</v>
       </c>
       <c r="L18" t="s">
-        <v>212</v>
+        <v>242</v>
       </c>
       <c r="M18" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N18">
         <v>18200</v>
@@ -3377,7 +3769,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B19" t="s">
         <v>81</v>
@@ -3392,10 +3784,10 @@
         <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G19" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -3404,16 +3796,16 @@
         <v>85</v>
       </c>
       <c r="J19" t="s">
-        <v>211</v>
+        <v>241</v>
       </c>
       <c r="K19">
         <v>7</v>
       </c>
       <c r="L19" t="s">
-        <v>213</v>
+        <v>243</v>
       </c>
       <c r="M19" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N19">
         <v>9800</v>
@@ -3421,7 +3813,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B20" t="s">
         <v>81</v>
@@ -3436,10 +3828,10 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G20" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
@@ -3448,16 +3840,16 @@
         <v>34</v>
       </c>
       <c r="J20" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="K20">
         <v>5</v>
       </c>
       <c r="L20" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="M20" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N20">
         <v>6750</v>
@@ -3465,7 +3857,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
@@ -3480,28 +3872,28 @@
         <v>36</v>
       </c>
       <c r="F21" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G21" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H21" t="s">
         <v>26</v>
       </c>
       <c r="I21" t="s">
-        <v>182</v>
+        <v>212</v>
       </c>
       <c r="J21" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="K21">
         <v>15</v>
       </c>
       <c r="L21" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
       <c r="M21" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N21">
         <v>20250</v>
@@ -3509,7 +3901,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B22" t="s">
         <v>89</v>
@@ -3524,10 +3916,10 @@
         <v>95</v>
       </c>
       <c r="F22" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G22" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H22" t="s">
         <v>26</v>
@@ -3536,16 +3928,16 @@
         <v>93</v>
       </c>
       <c r="J22" t="s">
-        <v>214</v>
+        <v>244</v>
       </c>
       <c r="K22">
         <v>11</v>
       </c>
       <c r="L22" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="M22" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N22">
         <v>14850</v>
@@ -3553,7 +3945,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B23" t="s">
         <v>89</v>
@@ -3568,28 +3960,28 @@
         <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G23" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H23" t="s">
         <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>215</v>
+        <v>245</v>
       </c>
       <c r="J23" t="s">
-        <v>216</v>
+        <v>246</v>
       </c>
       <c r="K23">
         <v>8</v>
       </c>
       <c r="L23" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="M23" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N23">
         <v>10800</v>
@@ -3597,7 +3989,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B24" t="s">
         <v>89</v>
@@ -3612,10 +4004,10 @@
         <v>52</v>
       </c>
       <c r="F24" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G24" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H24" t="s">
         <v>26</v>
@@ -3624,16 +4016,16 @@
         <v>98</v>
       </c>
       <c r="J24" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="K24">
         <v>11</v>
       </c>
       <c r="L24" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="M24" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N24">
         <v>14850</v>
@@ -3641,7 +4033,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B25" t="s">
         <v>89</v>
@@ -3656,28 +4048,28 @@
         <v>52</v>
       </c>
       <c r="F25" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="G25" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H25" t="s">
         <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>218</v>
+        <v>248</v>
       </c>
       <c r="J25" t="s">
-        <v>219</v>
+        <v>249</v>
       </c>
       <c r="K25">
         <v>8</v>
       </c>
       <c r="L25" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
       <c r="M25" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N25">
         <v>10800</v>
@@ -3685,7 +4077,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B26" t="s">
         <v>89</v>
@@ -3700,10 +4092,10 @@
         <v>52</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G26" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H26" t="s">
         <v>26</v>
@@ -3712,16 +4104,16 @@
         <v>103</v>
       </c>
       <c r="J26" t="s">
-        <v>220</v>
+        <v>250</v>
       </c>
       <c r="K26">
         <v>17</v>
       </c>
       <c r="L26" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="M26" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N26">
         <v>22950</v>
@@ -3729,7 +4121,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B27" t="s">
         <v>89</v>
@@ -3744,28 +4136,28 @@
         <v>52</v>
       </c>
       <c r="F27" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G27" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H27" t="s">
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>221</v>
+        <v>251</v>
       </c>
       <c r="J27" t="s">
-        <v>222</v>
+        <v>252</v>
       </c>
       <c r="K27">
         <v>2</v>
       </c>
       <c r="L27" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="M27" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N27">
         <v>2700</v>
@@ -3773,7 +4165,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B28" t="s">
         <v>89</v>
@@ -3788,10 +4180,10 @@
         <v>113</v>
       </c>
       <c r="F28" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="G28" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H28" t="s">
         <v>109</v>
@@ -3800,16 +4192,16 @@
         <v>108</v>
       </c>
       <c r="J28" t="s">
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="K28">
         <v>28</v>
       </c>
       <c r="L28" t="s">
-        <v>226</v>
+        <v>256</v>
       </c>
       <c r="M28" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="N28">
         <v>33600</v>
@@ -3817,7 +4209,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
@@ -3832,10 +4224,10 @@
         <v>119</v>
       </c>
       <c r="F29" t="s">
-        <v>223</v>
+        <v>253</v>
       </c>
       <c r="G29" t="s">
-        <v>224</v>
+        <v>254</v>
       </c>
       <c r="H29" t="s">
         <v>109</v>
@@ -3844,16 +4236,16 @@
         <v>117</v>
       </c>
       <c r="J29" t="s">
-        <v>228</v>
+        <v>258</v>
       </c>
       <c r="K29">
         <v>26</v>
       </c>
       <c r="L29" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="M29" t="s">
-        <v>227</v>
+        <v>257</v>
       </c>
       <c r="N29">
         <v>31200</v>
@@ -3861,7 +4253,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B30" t="s">
         <v>89</v>
@@ -3876,10 +4268,10 @@
         <v>125</v>
       </c>
       <c r="F30" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G30" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H30" t="s">
         <v>26</v>
@@ -3888,16 +4280,16 @@
         <v>123</v>
       </c>
       <c r="J30" t="s">
-        <v>230</v>
+        <v>260</v>
       </c>
       <c r="K30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>231</v>
+        <v>261</v>
       </c>
       <c r="M30" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N30">
         <v>5400</v>
@@ -3905,7 +4297,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
         <v>89</v>
@@ -3920,28 +4312,28 @@
         <v>125</v>
       </c>
       <c r="F31" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G31" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H31" t="s">
         <v>26</v>
       </c>
       <c r="I31" t="s">
-        <v>232</v>
+        <v>262</v>
       </c>
       <c r="J31" t="s">
-        <v>233</v>
+        <v>263</v>
       </c>
       <c r="K31">
         <v>18</v>
       </c>
       <c r="L31" t="s">
-        <v>234</v>
+        <v>264</v>
       </c>
       <c r="M31" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N31">
         <v>24300</v>
@@ -3949,7 +4341,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B32" t="s">
         <v>89</v>
@@ -3964,10 +4356,10 @@
         <v>52</v>
       </c>
       <c r="F32" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G32" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H32" t="s">
         <v>26</v>
@@ -3976,16 +4368,16 @@
         <v>127</v>
       </c>
       <c r="J32" t="s">
-        <v>235</v>
+        <v>265</v>
       </c>
       <c r="K32">
         <v>4</v>
       </c>
       <c r="L32" t="s">
-        <v>236</v>
+        <v>266</v>
       </c>
       <c r="M32" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N32">
         <v>5400</v>
@@ -3993,7 +4385,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B33" t="s">
         <v>89</v>
@@ -4008,28 +4400,28 @@
         <v>52</v>
       </c>
       <c r="F33" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G33" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H33" t="s">
         <v>26</v>
       </c>
       <c r="I33" t="s">
-        <v>237</v>
+        <v>267</v>
       </c>
       <c r="J33" t="s">
-        <v>238</v>
+        <v>268</v>
       </c>
       <c r="K33">
         <v>15</v>
       </c>
       <c r="L33" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="M33" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N33">
         <v>20250</v>
@@ -4037,7 +4429,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B34" t="s">
         <v>128</v>
@@ -4052,10 +4444,10 @@
         <v>95</v>
       </c>
       <c r="F34" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G34" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H34" t="s">
         <v>26</v>
@@ -4064,16 +4456,16 @@
         <v>130</v>
       </c>
       <c r="J34" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K34">
         <v>19</v>
       </c>
       <c r="L34" t="s">
-        <v>240</v>
+        <v>270</v>
       </c>
       <c r="M34" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N34">
         <v>25650</v>
@@ -4081,7 +4473,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B35" t="s">
         <v>128</v>
@@ -4096,10 +4488,10 @@
         <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G35" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H35" t="s">
         <v>26</v>
@@ -4108,16 +4500,16 @@
         <v>134</v>
       </c>
       <c r="J35" t="s">
-        <v>241</v>
+        <v>271</v>
       </c>
       <c r="K35">
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>195</v>
+        <v>225</v>
       </c>
       <c r="M35" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N35">
         <v>32400</v>
@@ -4125,7 +4517,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B36" t="s">
         <v>137</v>
@@ -4140,10 +4532,10 @@
         <v>52</v>
       </c>
       <c r="F36" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G36" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H36" t="s">
         <v>26</v>
@@ -4152,16 +4544,16 @@
         <v>140</v>
       </c>
       <c r="J36" t="s">
-        <v>242</v>
+        <v>272</v>
       </c>
       <c r="K36">
         <v>15</v>
       </c>
       <c r="L36" t="s">
-        <v>205</v>
+        <v>235</v>
       </c>
       <c r="M36" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N36">
         <v>20250</v>
@@ -4169,7 +4561,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B37" t="s">
         <v>137</v>
@@ -4184,28 +4576,28 @@
         <v>52</v>
       </c>
       <c r="F37" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G37" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H37" t="s">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>243</v>
+        <v>273</v>
       </c>
       <c r="J37" t="s">
-        <v>244</v>
+        <v>274</v>
       </c>
       <c r="K37">
         <v>4</v>
       </c>
       <c r="L37" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="M37" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N37">
         <v>5400</v>
@@ -4213,7 +4605,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
         <v>128</v>
@@ -4228,10 +4620,10 @@
         <v>148</v>
       </c>
       <c r="F38" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G38" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H38" t="s">
         <v>145</v>
@@ -4240,16 +4632,16 @@
         <v>144</v>
       </c>
       <c r="J38" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K38">
         <v>16</v>
       </c>
       <c r="L38" t="s">
-        <v>245</v>
+        <v>275</v>
       </c>
       <c r="M38" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="N38">
         <v>19600</v>
@@ -4257,7 +4649,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
         <v>128</v>
@@ -4272,10 +4664,10 @@
         <v>148</v>
       </c>
       <c r="F39" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G39" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H39" t="s">
         <v>145</v>
@@ -4284,16 +4676,16 @@
         <v>144</v>
       </c>
       <c r="J39" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K39">
         <v>8</v>
       </c>
       <c r="L39" t="s">
-        <v>247</v>
+        <v>277</v>
       </c>
       <c r="M39" t="s">
-        <v>246</v>
+        <v>276</v>
       </c>
       <c r="N39">
         <v>9800</v>
@@ -4301,7 +4693,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B40" t="s">
         <v>128</v>
@@ -4316,10 +4708,10 @@
         <v>155</v>
       </c>
       <c r="F40" t="s">
-        <v>248</v>
+        <v>278</v>
       </c>
       <c r="G40" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="H40" t="s">
         <v>145</v>
@@ -4328,16 +4720,16 @@
         <v>152</v>
       </c>
       <c r="J40" t="s">
-        <v>239</v>
+        <v>269</v>
       </c>
       <c r="K40">
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>249</v>
+        <v>279</v>
       </c>
       <c r="M40" t="s">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="N40">
         <v>28800</v>
@@ -4345,7 +4737,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B41" t="s">
         <v>128</v>
@@ -4360,10 +4752,10 @@
         <v>125</v>
       </c>
       <c r="F41" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="G41" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="H41" t="s">
         <v>26</v>
@@ -4372,19 +4764,547 @@
         <v>159</v>
       </c>
       <c r="J41" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="K41">
         <v>22</v>
       </c>
       <c r="L41" t="s">
-        <v>251</v>
+        <v>281</v>
       </c>
       <c r="M41" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
       <c r="N41">
         <v>29700</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>201</v>
+      </c>
+      <c r="B42" t="s">
+        <v>128</v>
+      </c>
+      <c r="C42" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F42" t="s">
+        <v>202</v>
+      </c>
+      <c r="G42" t="s">
+        <v>203</v>
+      </c>
+      <c r="H42" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42" t="s">
+        <v>164</v>
+      </c>
+      <c r="J42" t="s">
+        <v>282</v>
+      </c>
+      <c r="K42">
+        <v>22</v>
+      </c>
+      <c r="L42" t="s">
+        <v>281</v>
+      </c>
+      <c r="M42" t="s">
+        <v>216</v>
+      </c>
+      <c r="N42">
+        <v>29700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>201</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>28</v>
+      </c>
+      <c r="E43" t="s">
+        <v>52</v>
+      </c>
+      <c r="F43" t="s">
+        <v>202</v>
+      </c>
+      <c r="G43" t="s">
+        <v>203</v>
+      </c>
+      <c r="H43" t="s">
+        <v>26</v>
+      </c>
+      <c r="I43" t="s">
+        <v>170</v>
+      </c>
+      <c r="J43" t="s">
+        <v>283</v>
+      </c>
+      <c r="K43">
+        <v>19</v>
+      </c>
+      <c r="L43" t="s">
+        <v>235</v>
+      </c>
+      <c r="M43" t="s">
+        <v>216</v>
+      </c>
+      <c r="N43">
+        <v>25650</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F44" t="s">
+        <v>202</v>
+      </c>
+      <c r="G44" t="s">
+        <v>203</v>
+      </c>
+      <c r="H44" t="s">
+        <v>26</v>
+      </c>
+      <c r="I44" t="s">
+        <v>173</v>
+      </c>
+      <c r="J44" t="s">
+        <v>284</v>
+      </c>
+      <c r="K44">
+        <v>6</v>
+      </c>
+      <c r="L44" t="s">
+        <v>266</v>
+      </c>
+      <c r="M44" t="s">
+        <v>206</v>
+      </c>
+      <c r="N44">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>201</v>
+      </c>
+      <c r="B45" t="s">
+        <v>166</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" t="s">
+        <v>95</v>
+      </c>
+      <c r="F45" t="s">
+        <v>202</v>
+      </c>
+      <c r="G45" t="s">
+        <v>203</v>
+      </c>
+      <c r="H45" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" t="s">
+        <v>285</v>
+      </c>
+      <c r="J45" t="s">
+        <v>286</v>
+      </c>
+      <c r="K45">
+        <v>13</v>
+      </c>
+      <c r="L45" t="s">
+        <v>287</v>
+      </c>
+      <c r="M45" t="s">
+        <v>206</v>
+      </c>
+      <c r="N45">
+        <v>17550</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>201</v>
+      </c>
+      <c r="B46" t="s">
+        <v>166</v>
+      </c>
+      <c r="C46" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" t="s">
+        <v>202</v>
+      </c>
+      <c r="G46" t="s">
+        <v>203</v>
+      </c>
+      <c r="H46" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" t="s">
+        <v>177</v>
+      </c>
+      <c r="J46" t="s">
+        <v>288</v>
+      </c>
+      <c r="K46">
+        <v>7</v>
+      </c>
+      <c r="L46" t="s">
+        <v>287</v>
+      </c>
+      <c r="M46" t="s">
+        <v>206</v>
+      </c>
+      <c r="N46">
+        <v>9450</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>201</v>
+      </c>
+      <c r="B47" t="s">
+        <v>166</v>
+      </c>
+      <c r="C47" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" t="s">
+        <v>202</v>
+      </c>
+      <c r="G47" t="s">
+        <v>203</v>
+      </c>
+      <c r="H47" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" t="s">
+        <v>289</v>
+      </c>
+      <c r="J47" t="s">
+        <v>290</v>
+      </c>
+      <c r="K47">
+        <v>12</v>
+      </c>
+      <c r="L47" t="s">
+        <v>270</v>
+      </c>
+      <c r="M47" t="s">
+        <v>206</v>
+      </c>
+      <c r="N47">
+        <v>16200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>201</v>
+      </c>
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" t="s">
+        <v>202</v>
+      </c>
+      <c r="G48" t="s">
+        <v>203</v>
+      </c>
+      <c r="H48" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" t="s">
+        <v>182</v>
+      </c>
+      <c r="J48" t="s">
+        <v>291</v>
+      </c>
+      <c r="K48">
+        <v>5</v>
+      </c>
+      <c r="L48" t="s">
+        <v>292</v>
+      </c>
+      <c r="M48" t="s">
+        <v>216</v>
+      </c>
+      <c r="N48">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>201</v>
+      </c>
+      <c r="B49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C49" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" t="s">
+        <v>202</v>
+      </c>
+      <c r="G49" t="s">
+        <v>203</v>
+      </c>
+      <c r="H49" t="s">
+        <v>26</v>
+      </c>
+      <c r="I49" t="s">
+        <v>293</v>
+      </c>
+      <c r="J49" t="s">
+        <v>294</v>
+      </c>
+      <c r="K49">
+        <v>15</v>
+      </c>
+      <c r="L49" t="s">
+        <v>225</v>
+      </c>
+      <c r="M49" t="s">
+        <v>216</v>
+      </c>
+      <c r="N49">
+        <v>20250</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>201</v>
+      </c>
+      <c r="B50" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" t="s">
+        <v>75</v>
+      </c>
+      <c r="D50" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+      <c r="F50" t="s">
+        <v>202</v>
+      </c>
+      <c r="G50" t="s">
+        <v>203</v>
+      </c>
+      <c r="H50" t="s">
+        <v>26</v>
+      </c>
+      <c r="I50" t="s">
+        <v>185</v>
+      </c>
+      <c r="J50" t="s">
+        <v>295</v>
+      </c>
+      <c r="K50">
+        <v>5</v>
+      </c>
+      <c r="L50" t="s">
+        <v>233</v>
+      </c>
+      <c r="M50" t="s">
+        <v>206</v>
+      </c>
+      <c r="N50">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>201</v>
+      </c>
+      <c r="B51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" t="s">
+        <v>203</v>
+      </c>
+      <c r="H51" t="s">
+        <v>26</v>
+      </c>
+      <c r="I51" t="s">
+        <v>296</v>
+      </c>
+      <c r="J51" t="s">
+        <v>297</v>
+      </c>
+      <c r="K51">
+        <v>14</v>
+      </c>
+      <c r="L51" t="s">
+        <v>235</v>
+      </c>
+      <c r="M51" t="s">
+        <v>206</v>
+      </c>
+      <c r="N51">
+        <v>18900</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>201</v>
+      </c>
+      <c r="B52" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" t="s">
+        <v>28</v>
+      </c>
+      <c r="E52" t="s">
+        <v>95</v>
+      </c>
+      <c r="F52" t="s">
+        <v>202</v>
+      </c>
+      <c r="G52" t="s">
+        <v>203</v>
+      </c>
+      <c r="H52" t="s">
+        <v>26</v>
+      </c>
+      <c r="I52" t="s">
+        <v>189</v>
+      </c>
+      <c r="J52" t="s">
+        <v>298</v>
+      </c>
+      <c r="K52">
+        <v>8</v>
+      </c>
+      <c r="L52" t="s">
+        <v>233</v>
+      </c>
+      <c r="M52" t="s">
+        <v>206</v>
+      </c>
+      <c r="N52">
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C53" t="s">
+        <v>190</v>
+      </c>
+      <c r="D53" t="s">
+        <v>28</v>
+      </c>
+      <c r="E53" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" t="s">
+        <v>202</v>
+      </c>
+      <c r="G53" t="s">
+        <v>203</v>
+      </c>
+      <c r="H53" t="s">
+        <v>26</v>
+      </c>
+      <c r="I53" t="s">
+        <v>299</v>
+      </c>
+      <c r="J53" t="s">
+        <v>300</v>
+      </c>
+      <c r="K53">
+        <v>11</v>
+      </c>
+      <c r="L53" t="s">
+        <v>235</v>
+      </c>
+      <c r="M53" t="s">
+        <v>206</v>
+      </c>
+      <c r="N53">
+        <v>14850</v>
       </c>
     </row>
   </sheetData>
@@ -4427,7 +5347,7 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
       <c r="F2" s="32" t="s">
-        <v>252</v>
+        <v>301</v>
       </c>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
@@ -4515,22 +5435,22 @@
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
-        <v>253</v>
+        <v>302</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="34" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="3"/>
       <c r="H8" s="9" t="s">
-        <v>254</v>
+        <v>303</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="3"/>
       <c r="K8" s="35" t="s">
-        <v>156</v>
+        <v>186</v>
       </c>
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
@@ -4559,11 +5479,11 @@
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
-        <v>255</v>
+        <v>304</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="13" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -4599,11 +5519,11 @@
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>256</v>
+        <v>305</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="13" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -4639,22 +5559,22 @@
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="17" t="s">
-        <v>257</v>
+        <v>306</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="13" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="3"/>
       <c r="H14" s="9" t="s">
-        <v>258</v>
+        <v>307</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="3"/>
       <c r="K14" s="13" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -4683,11 +5603,11 @@
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
-        <v>259</v>
+        <v>308</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="13" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -4723,7 +5643,7 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
-        <v>260</v>
+        <v>309</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="13" t="s">
@@ -4735,12 +5655,12 @@
       <c r="H18" s="7"/>
       <c r="I18" s="3"/>
       <c r="J18" s="9" t="s">
-        <v>261</v>
+        <v>310</v>
       </c>
       <c r="K18" s="7"/>
       <c r="L18" s="3"/>
       <c r="M18" s="13" t="s">
-        <v>173</v>
+        <v>203</v>
       </c>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
@@ -4767,31 +5687,31 @@
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="17" t="s">
-        <v>262</v>
+        <v>311</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="13" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="3"/>
       <c r="H20" s="15" t="s">
-        <v>263</v>
+        <v>312</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="3"/>
       <c r="K20" s="13" t="s">
-        <v>250</v>
+        <v>298</v>
       </c>
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
       <c r="N20" s="3"/>
       <c r="O20" s="17" t="s">
-        <v>264</v>
+        <v>313</v>
       </c>
       <c r="P20" s="13">
-        <v>29700</v>
+        <v>10800</v>
       </c>
       <c r="Q20" s="3"/>
     </row>
@@ -4815,31 +5735,31 @@
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="17" t="s">
-        <v>265</v>
+        <v>314</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="13" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="3"/>
       <c r="H22" s="15" t="s">
-        <v>267</v>
+        <v>315</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="3"/>
       <c r="K22" s="13" t="s">
-        <v>266</v>
+        <v>300</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="3"/>
       <c r="O22" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="P22" s="13" t="s">
-        <v>266</v>
+        <v>316</v>
+      </c>
+      <c r="P22" s="13">
+        <v>14850</v>
       </c>
       <c r="Q22" s="3"/>
     </row>
@@ -4863,31 +5783,31 @@
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="17" t="s">
-        <v>269</v>
+        <v>317</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="3"/>
       <c r="H24" s="15" t="s">
-        <v>270</v>
+        <v>319</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="3"/>
       <c r="K24" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
       <c r="N24" s="3"/>
       <c r="O24" s="17" t="s">
-        <v>271</v>
+        <v>320</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="Q24" s="3"/>
     </row>
@@ -4911,11 +5831,11 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
-        <v>272</v>
+        <v>321</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="13" t="s">
-        <v>172</v>
+        <v>202</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -4923,11 +5843,11 @@
       <c r="H26" s="7"/>
       <c r="I26" s="3"/>
       <c r="J26" s="9" t="s">
-        <v>273</v>
+        <v>322</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="30" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -4955,11 +5875,11 @@
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="13" t="s">
-        <v>251</v>
+        <v>233</v>
       </c>
       <c r="E28" s="15" t="s">
         <v>4</v>
@@ -4967,25 +5887,25 @@
       <c r="F28" s="7"/>
       <c r="G28" s="3"/>
       <c r="H28" s="13" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
       <c r="J28" s="3"/>
       <c r="K28" s="13">
-        <v>29700</v>
+        <v>10800</v>
       </c>
       <c r="L28" s="3"/>
       <c r="M28" s="6" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="13">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="P28" s="16" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
       <c r="Q28" s="33"/>
     </row>
@@ -5009,11 +5929,11 @@
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="13" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="E30" s="15" t="s">
         <v>4</v>
@@ -5021,25 +5941,25 @@
       <c r="F30" s="7"/>
       <c r="G30" s="3"/>
       <c r="H30" s="13" t="s">
-        <v>266</v>
+        <v>299</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="13" t="s">
-        <v>266</v>
+      <c r="K30" s="13">
+        <v>14850</v>
       </c>
       <c r="L30" s="3"/>
       <c r="M30" s="6" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
       <c r="N30" s="7"/>
-      <c r="O30" s="13" t="s">
-        <v>266</v>
+      <c r="O30" s="13">
+        <v>11</v>
       </c>
       <c r="P30" s="16" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
       <c r="Q30" s="33"/>
     </row>
@@ -5063,11 +5983,11 @@
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="E32" s="15" t="s">
         <v>4</v>
@@ -5075,25 +5995,25 @@
       <c r="F32" s="7"/>
       <c r="G32" s="3"/>
       <c r="H32" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>275</v>
+        <v>324</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="L32" s="3"/>
       <c r="M32" s="6" t="s">
-        <v>276</v>
+        <v>325</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="13" t="s">
-        <v>266</v>
+        <v>318</v>
       </c>
       <c r="P32" s="16" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
       <c r="Q32" s="13"/>
     </row>
@@ -5118,7 +6038,7 @@
     <row r="34" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="32" t="s">
-        <v>278</v>
+        <v>327</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
@@ -5156,12 +6076,12 @@
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
-        <v>279</v>
+        <v>328</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="13"/>
       <c r="E38" s="15" t="s">
-        <v>280</v>
+        <v>329</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="3"/>
@@ -5169,7 +6089,7 @@
       <c r="I38" s="7"/>
       <c r="J38" s="3"/>
       <c r="K38" s="15" t="s">
-        <v>281</v>
+        <v>330</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="9"/>
@@ -5198,12 +6118,12 @@
     </row>
     <row r="40" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
-        <v>282</v>
+        <v>331</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="13"/>
       <c r="E40" s="29" t="s">
-        <v>283</v>
+        <v>332</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="3"/>
@@ -5211,7 +6131,7 @@
       <c r="I40" s="7"/>
       <c r="J40" s="3"/>
       <c r="K40" s="2" t="s">
-        <v>284</v>
+        <v>333</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="9"/>
@@ -5240,7 +6160,7 @@
     </row>
     <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="15" t="s">
-        <v>285</v>
+        <v>334</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="13"/>
@@ -5251,7 +6171,7 @@
       <c r="I42" s="7"/>
       <c r="J42" s="3"/>
       <c r="K42" s="15" t="s">
-        <v>286</v>
+        <v>335</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="13"/>
@@ -5280,23 +6200,23 @@
     </row>
     <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>287</v>
+        <v>336</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="19" t="s">
-        <v>288</v>
+        <v>337</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="3"/>
       <c r="G44" s="18" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="9"/>
       <c r="J44" s="7"/>
       <c r="K44" s="3"/>
       <c r="L44" s="15" t="s">
-        <v>290</v>
+        <v>339</v>
       </c>
       <c r="M44" s="7"/>
       <c r="N44" s="7"/>
@@ -5329,14 +6249,14 @@
       <c r="E46" s="4"/>
       <c r="F46" s="5"/>
       <c r="G46" s="18" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="H46" s="3"/>
       <c r="I46" s="9"/>
       <c r="J46" s="7"/>
       <c r="K46" s="3"/>
       <c r="L46" s="15" t="s">
-        <v>290</v>
+        <v>339</v>
       </c>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
@@ -5348,7 +6268,7 @@
       <c r="B47" s="11"/>
       <c r="C47" s="12"/>
       <c r="D47" s="19" t="s">
-        <v>291</v>
+        <v>340</v>
       </c>
       <c r="E47" s="7"/>
       <c r="F47" s="3"/>
@@ -5371,14 +6291,14 @@
       <c r="E48" s="20"/>
       <c r="F48" s="12"/>
       <c r="G48" s="18" t="s">
-        <v>289</v>
+        <v>338</v>
       </c>
       <c r="H48" s="3"/>
       <c r="I48" s="9"/>
       <c r="J48" s="7"/>
       <c r="K48" s="3"/>
       <c r="L48" s="15" t="s">
-        <v>290</v>
+        <v>339</v>
       </c>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
@@ -5407,7 +6327,7 @@
     <row r="50" spans="2:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B51" s="31" t="s">
-        <v>292</v>
+        <v>341</v>
       </c>
       <c r="C51" s="22"/>
       <c r="D51" s="22"/>

</xml_diff>

<commit_message>
separando o comando de salvar dados da interface
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -802,7 +802,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:XFD26"/>
@@ -2970,6 +2970,171 @@
         </is>
       </c>
     </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>516</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>516</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>516</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2981,7 +3146,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD41"/>
@@ -7155,6 +7320,414 @@
       </c>
       <c r="N61" t="n">
         <v>652</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>150561</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>ddas</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>150561</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>ddas</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>5156</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>150561</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>ddas</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>5156</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>86415</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>6541</v>
       </c>
     </row>
   </sheetData>
@@ -7262,7 +7835,7 @@
       <c r="C8" s="3" t="n"/>
       <c r="D8" s="34" t="inlineStr">
         <is>
-          <t>adsd</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E8" s="7" t="n"/>
@@ -7515,7 +8088,7 @@
       <c r="L18" s="3" t="n"/>
       <c r="M18" s="13" t="inlineStr">
         <is>
-          <t>BIG BAG</t>
+          <t>Selecione uma opção</t>
         </is>
       </c>
       <c r="N18" s="7" t="n"/>
@@ -7577,7 +8150,7 @@
         </is>
       </c>
       <c r="P20" s="13" t="n">
-        <v>652</v>
+        <v>7413</v>
       </c>
       <c r="Q20" s="3" t="n"/>
     </row>
@@ -7780,7 +8353,7 @@
       <c r="C28" s="3" t="n"/>
       <c r="D28" s="13" t="inlineStr">
         <is>
-          <t>das</t>
+          <t>ddas</t>
         </is>
       </c>
       <c r="E28" s="15" t="inlineStr">
@@ -7802,7 +8375,7 @@
       </c>
       <c r="J28" s="3" t="n"/>
       <c r="K28" s="13" t="n">
-        <v>652</v>
+        <v>516</v>
       </c>
       <c r="L28" s="3" t="n"/>
       <c r="M28" s="6" t="inlineStr">
@@ -7812,7 +8385,7 @@
       </c>
       <c r="N28" s="7" t="n"/>
       <c r="O28" s="13" t="n">
-        <v>65</v>
+        <v>150561</v>
       </c>
       <c r="P28" s="16" t="inlineStr">
         <is>
@@ -7848,7 +8421,7 @@
       <c r="C30" s="3" t="n"/>
       <c r="D30" s="13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="E30" s="15" t="inlineStr">
@@ -7860,7 +8433,7 @@
       <c r="G30" s="3" t="n"/>
       <c r="H30" s="13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="I30" s="15" t="inlineStr">
@@ -7869,10 +8442,8 @@
         </is>
       </c>
       <c r="J30" s="3" t="n"/>
-      <c r="K30" s="13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="K30" s="13" t="n">
+        <v>356</v>
       </c>
       <c r="L30" s="3" t="n"/>
       <c r="M30" s="6" t="inlineStr">
@@ -7881,10 +8452,8 @@
         </is>
       </c>
       <c r="N30" s="7" t="n"/>
-      <c r="O30" s="13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="O30" s="13" t="n">
+        <v>5156</v>
       </c>
       <c r="P30" s="16" t="inlineStr">
         <is>
@@ -7920,7 +8489,7 @@
       <c r="C32" s="3" t="n"/>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="E32" s="15" t="inlineStr">
@@ -7932,7 +8501,7 @@
       <c r="G32" s="3" t="n"/>
       <c r="H32" s="13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="I32" s="15" t="inlineStr">
@@ -7941,10 +8510,8 @@
         </is>
       </c>
       <c r="J32" s="3" t="n"/>
-      <c r="K32" s="13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="K32" s="13" t="n">
+        <v>6541</v>
       </c>
       <c r="L32" s="3" t="n"/>
       <c r="M32" s="6" t="inlineStr">
@@ -7953,10 +8520,8 @@
         </is>
       </c>
       <c r="N32" s="7" t="n"/>
-      <c r="O32" s="13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="O32" s="13" t="n">
+        <v>86415</v>
       </c>
       <c r="P32" s="16" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
adicionado uma segunda aba
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -802,7 +802,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A26" sqref="A26:XFD26"/>
@@ -3135,6 +3135,226 @@
         </is>
       </c>
     </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>516</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>265</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>265</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>dasd</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>265</v>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>SAL REFINADO Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -3146,7 +3366,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N67"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A41" sqref="A41:XFD41"/>
@@ -7728,6 +7948,482 @@
       </c>
       <c r="N67" t="n">
         <v>6541</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>561</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>68</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>68</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K71" t="n">
+        <v>165</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K72" t="n">
+        <v>68</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>165</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>SAL REFINADO</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>NORSAL</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>145</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -7887,7 +8583,7 @@
       <c r="C10" s="3" t="n"/>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>das</t>
+          <t>dasd</t>
         </is>
       </c>
       <c r="E10" s="7" t="n"/>
@@ -8150,7 +8846,7 @@
         </is>
       </c>
       <c r="P20" s="13" t="n">
-        <v>7413</v>
+        <v>356</v>
       </c>
       <c r="Q20" s="3" t="n"/>
     </row>
@@ -8353,7 +9049,7 @@
       <c r="C28" s="3" t="n"/>
       <c r="D28" s="13" t="inlineStr">
         <is>
-          <t>ddas</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E28" s="15" t="inlineStr">
@@ -8375,7 +9071,7 @@
       </c>
       <c r="J28" s="3" t="n"/>
       <c r="K28" s="13" t="n">
-        <v>516</v>
+        <v>265</v>
       </c>
       <c r="L28" s="3" t="n"/>
       <c r="M28" s="6" t="inlineStr">
@@ -8385,7 +9081,7 @@
       </c>
       <c r="N28" s="7" t="n"/>
       <c r="O28" s="13" t="n">
-        <v>150561</v>
+        <v>68</v>
       </c>
       <c r="P28" s="16" t="inlineStr">
         <is>
@@ -8443,7 +9139,7 @@
       </c>
       <c r="J30" s="3" t="n"/>
       <c r="K30" s="13" t="n">
-        <v>356</v>
+        <v>65</v>
       </c>
       <c r="L30" s="3" t="n"/>
       <c r="M30" s="6" t="inlineStr">
@@ -8453,7 +9149,7 @@
       </c>
       <c r="N30" s="7" t="n"/>
       <c r="O30" s="13" t="n">
-        <v>5156</v>
+        <v>165</v>
       </c>
       <c r="P30" s="16" t="inlineStr">
         <is>
@@ -8511,7 +9207,7 @@
       </c>
       <c r="J32" s="3" t="n"/>
       <c r="K32" s="13" t="n">
-        <v>6541</v>
+        <v>26</v>
       </c>
       <c r="L32" s="3" t="n"/>
       <c r="M32" s="6" t="inlineStr">
@@ -8521,7 +9217,7 @@
       </c>
       <c r="N32" s="7" t="n"/>
       <c r="O32" s="13" t="n">
-        <v>86415</v>
+        <v>145</v>
       </c>
       <c r="P32" s="16" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
colocando os outros campos do produto na função
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -12854,7 +12854,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
@@ -13028,6 +13028,654 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>asdasx</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>saxsa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>asdasx</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>saxsa</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>xsa</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>xas</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>frv</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>rfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>yhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ikmik</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>ik</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>ikm</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>EMBALAGEM</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>dfg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>

</xml_diff>

<commit_message>
correção , erro funcional não salvava os dados da carga no espelho do sal
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -1378,7 +1378,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
@@ -1621,6 +1621,116 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>05:27</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>valdik antonio sa silva</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>sda</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>dsa/rte</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>651</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Selecione uma opção Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>das/dsa</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>379</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Selecione uma opção Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1632,7 +1742,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:N98"/>
@@ -2134,6 +2244,278 @@
       </c>
       <c r="N7" t="n">
         <v>234</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>84965</v>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N8" t="n">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>03/04/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>rte</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>98</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>8956</v>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>fe</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N9" t="n">
+        <v>98465</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>249</v>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ENTRADA</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Selecione uma opção</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>dsa</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="K11" t="n">
+        <v>2767</v>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>das</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>5786</v>
       </c>
     </row>
   </sheetData>
@@ -2241,7 +2623,7 @@
       <c r="C8" s="15" t="n"/>
       <c r="D8" s="46" t="inlineStr">
         <is>
-          <t>fdgf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E8" s="19" t="n"/>
@@ -2256,7 +2638,7 @@
       <c r="J8" s="15" t="n"/>
       <c r="K8" s="47" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="L8" s="19" t="n"/>
@@ -2293,7 +2675,7 @@
       <c r="C10" s="15" t="n"/>
       <c r="D10" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E10" s="19" t="n"/>
@@ -2337,7 +2719,7 @@
       <c r="C12" s="15" t="n"/>
       <c r="D12" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E12" s="19" t="n"/>
@@ -2381,7 +2763,7 @@
       <c r="C14" s="15" t="n"/>
       <c r="D14" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E14" s="19" t="n"/>
@@ -2396,7 +2778,7 @@
       <c r="J14" s="15" t="n"/>
       <c r="K14" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="L14" s="19" t="n"/>
@@ -2433,7 +2815,7 @@
       <c r="C16" s="15" t="n"/>
       <c r="D16" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E16" s="19" t="n"/>
@@ -2477,7 +2859,7 @@
       <c r="C18" s="15" t="n"/>
       <c r="D18" s="25" t="inlineStr">
         <is>
-          <t>NORSAL</t>
+          <t>Selecione uma opção</t>
         </is>
       </c>
       <c r="E18" s="19" t="n"/>
@@ -2529,7 +2911,7 @@
       <c r="C20" s="15" t="n"/>
       <c r="D20" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E20" s="19" t="n"/>
@@ -2544,7 +2926,7 @@
       <c r="J20" s="15" t="n"/>
       <c r="K20" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="L20" s="19" t="n"/>
@@ -2556,7 +2938,7 @@
         </is>
       </c>
       <c r="P20" s="25" t="n">
-        <v>702</v>
+        <v>379</v>
       </c>
       <c r="Q20" s="15" t="n"/>
     </row>
@@ -2587,7 +2969,7 @@
       <c r="C22" s="15" t="n"/>
       <c r="D22" s="25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>dsa</t>
         </is>
       </c>
       <c r="E22" s="19" t="n"/>
@@ -2602,7 +2984,7 @@
       <c r="J22" s="15" t="n"/>
       <c r="K22" s="25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="L22" s="19" t="n"/>
@@ -2613,10 +2995,8 @@
           <t>PESO NF 2:</t>
         </is>
       </c>
-      <c r="P22" s="25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="P22" s="25" t="n">
+        <v>5786</v>
       </c>
       <c r="Q22" s="15" t="n"/>
     </row>
@@ -2707,7 +3087,7 @@
       <c r="C26" s="15" t="n"/>
       <c r="D26" s="25" t="inlineStr">
         <is>
-          <t>SAL REFINADO</t>
+          <t>Selecione uma opção</t>
         </is>
       </c>
       <c r="E26" s="19" t="n"/>
@@ -2723,7 +3103,7 @@
       <c r="K26" s="15" t="n"/>
       <c r="L26" s="42" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="M26" s="19" t="n"/>
@@ -2759,7 +3139,7 @@
       <c r="C28" s="15" t="n"/>
       <c r="D28" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="E28" s="27" t="inlineStr">
@@ -2771,7 +3151,7 @@
       <c r="G28" s="15" t="n"/>
       <c r="H28" s="25" t="inlineStr">
         <is>
-          <t>gdf</t>
+          <t>das</t>
         </is>
       </c>
       <c r="I28" s="27" t="inlineStr">
@@ -2781,7 +3161,7 @@
       </c>
       <c r="J28" s="15" t="n"/>
       <c r="K28" s="25" t="n">
-        <v>234</v>
+        <v>379</v>
       </c>
       <c r="L28" s="15" t="n"/>
       <c r="M28" s="18" t="inlineStr">
@@ -2791,7 +3171,7 @@
       </c>
       <c r="N28" s="19" t="n"/>
       <c r="O28" s="25" t="n">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="P28" s="28" t="inlineStr">
         <is>
@@ -2827,7 +3207,7 @@
       <c r="C30" s="15" t="n"/>
       <c r="D30" s="25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>das</t>
         </is>
       </c>
       <c r="E30" s="27" t="inlineStr">
@@ -2839,7 +3219,7 @@
       <c r="G30" s="15" t="n"/>
       <c r="H30" s="25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>dsa</t>
         </is>
       </c>
       <c r="I30" s="27" t="inlineStr">
@@ -2848,10 +3228,8 @@
         </is>
       </c>
       <c r="J30" s="15" t="n"/>
-      <c r="K30" s="25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="K30" s="25" t="n">
+        <v>5786</v>
       </c>
       <c r="L30" s="15" t="n"/>
       <c r="M30" s="18" t="inlineStr">
@@ -2860,10 +3238,8 @@
         </is>
       </c>
       <c r="N30" s="19" t="n"/>
-      <c r="O30" s="25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+      <c r="O30" s="25" t="n">
+        <v>2767</v>
       </c>
       <c r="P30" s="28" t="inlineStr">
         <is>

</xml_diff>